<commit_message>
fixed numbers for HIsarna energy use
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_var.xlsx
+++ b/data/steel/steel_simplified_var.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A686CC9-4B08-D845-B99A-3028541D7C1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A06CA14-EBC4-7B4B-AF31-B662BE049896}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="460" windowWidth="18540" windowHeight="17540" tabRatio="598" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2380" yWindow="460" windowWidth="18540" windowHeight="17540" tabRatio="598" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="17" r:id="rId1"/>
@@ -50,7 +50,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>S.E. Tanzer</author>
-    <author>Microsoft Office User</author>
   </authors>
   <commentList>
     <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
@@ -112,48 +111,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Zhang et al - </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>doi:10.1088/1755-1315/233/5/052016</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -204,7 +161,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -213,12 +170,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Following IEA 2007 - https://www.iea.org/publications/freepublications/publication/tracking_emissions.pdf
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Following IEA 2007 - https://www.iea.org/publications/freepublications/publication/tracking_emissions.pdf
 </t>
         </r>
       </text>
@@ -2724,7 +2690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -7057,7 +7023,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7663,7 +7629,7 @@
         <v>113</v>
       </c>
       <c r="M11" s="47">
-        <v>0.56000000000000005</v>
+        <v>0.61</v>
       </c>
       <c r="N11" s="42" t="s">
         <v>118</v>
@@ -7683,7 +7649,7 @@
       </c>
       <c r="S11" s="75">
         <f t="shared" si="4"/>
-        <v>14.448000000000002</v>
+        <v>15.738</v>
       </c>
       <c r="T11" s="42"/>
     </row>
@@ -7734,9 +7700,8 @@
         <f t="shared" si="6"/>
         <v>charcoal - IPCC</v>
       </c>
-      <c r="M12" s="90">
-        <f>M11</f>
-        <v>0.56000000000000005</v>
+      <c r="M12" s="47">
+        <v>0.61</v>
       </c>
       <c r="N12" s="26" t="str">
         <f t="shared" si="6"/>
@@ -7753,7 +7718,7 @@
       <c r="R12" s="81"/>
       <c r="S12" s="65">
         <f t="shared" si="4"/>
-        <v>14.448000000000002</v>
+        <v>15.738</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -7803,9 +7768,8 @@
         <f t="shared" si="7"/>
         <v>charcoal - IPCC</v>
       </c>
-      <c r="M13" s="41">
-        <f>M11</f>
-        <v>0.56000000000000005</v>
+      <c r="M13" s="47">
+        <v>0.61</v>
       </c>
       <c r="N13" s="21" t="str">
         <f t="shared" si="7"/>
@@ -7822,7 +7786,7 @@
       <c r="R13" s="81"/>
       <c r="S13" s="65">
         <f t="shared" si="4"/>
-        <v>14.448000000000002</v>
+        <v>15.738</v>
       </c>
       <c r="T13" s="21"/>
     </row>
@@ -7851,6 +7815,12 @@
       <c r="R17" s="81"/>
       <c r="S17" s="55"/>
       <c r="T17" s="21"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H18" s="27">
+        <f>H11/Ref!C12</f>
+        <v>749.37546149359912</v>
+      </c>
     </row>
     <row r="21" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21"/>
@@ -9475,7 +9445,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9741,8 +9711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
removed electricity heat recycling from BBF
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_var.xlsx
+++ b/data/steel/steel_simplified_var.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FC7E9F-A834-FF42-9AE2-44BA3BE2EB85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56F615F-3FFD-C44F-9322-3A945A349B80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="598" firstSheet="1" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="598" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="17" r:id="rId1"/>
@@ -1301,7 +1301,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1477,6 +1477,9 @@
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2705,7 +2708,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3498,8 +3501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3567,7 +3570,7 @@
       </c>
       <c r="C4" s="10">
         <f>C8</f>
-        <v>0.81069042316258355</v>
+        <v>0</v>
       </c>
       <c r="D4" s="54" t="s">
         <v>95</v>
@@ -3628,9 +3631,8 @@
       <c r="B8" s="82">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C8" s="47">
-        <f>1-(0.85/(0.85+0.66+2.98))</f>
-        <v>0.81069042316258355</v>
+      <c r="C8" s="141">
+        <v>0</v>
       </c>
       <c r="D8" s="82" t="s">
         <v>95</v>
@@ -3643,9 +3645,9 @@
       <c r="B9" s="82">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="142">
         <f t="shared" ref="C9" si="0">C$8</f>
-        <v>0.81069042316258355</v>
+        <v>0</v>
       </c>
       <c r="D9" s="21" t="str">
         <f>D8</f>
@@ -3659,9 +3661,9 @@
       <c r="B10" s="83">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="143">
         <f t="shared" ref="C10:D10" si="1">C$8</f>
-        <v>0.81069042316258355</v>
+        <v>0</v>
       </c>
       <c r="D10" s="45" t="str">
         <f t="shared" si="1"/>
@@ -3675,7 +3677,7 @@
       <c r="B11" s="82">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="141">
         <v>0</v>
       </c>
       <c r="D11" s="82" t="s">
@@ -3696,7 +3698,7 @@
         <f>B11</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="142">
         <f>C11</f>
         <v>0</v>
       </c>
@@ -3719,7 +3721,7 @@
         <f>B11</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="143">
         <f>C11</f>
         <v>0</v>
       </c>
@@ -3741,7 +3743,7 @@
       <c r="B14" s="82">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="141">
         <v>0</v>
       </c>
       <c r="D14" s="82" t="s">
@@ -3762,7 +3764,7 @@
         <f>B14</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="142">
         <f>C14</f>
         <v>0</v>
       </c>
@@ -3785,7 +3787,7 @@
         <f>B14</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="143">
         <f>C14</f>
         <v>0</v>
       </c>
@@ -3807,7 +3809,7 @@
       <c r="B17" s="82">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="141">
         <v>0</v>
       </c>
       <c r="D17" s="82" t="s">
@@ -3828,7 +3830,7 @@
         <f>B17</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="142">
         <f>C17</f>
         <v>0</v>
       </c>
@@ -3851,7 +3853,7 @@
         <f>B17</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="143">
         <f>C17</f>
         <v>0</v>
       </c>
@@ -3873,7 +3875,7 @@
       <c r="B20" s="82">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="141">
         <v>0</v>
       </c>
       <c r="D20" s="82" t="s">
@@ -3894,7 +3896,7 @@
         <f>B20</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="142">
         <f>C20</f>
         <v>0</v>
       </c>
@@ -3917,7 +3919,7 @@
         <f>B20</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="143">
         <f>C20</f>
         <v>0</v>
       </c>
@@ -4623,7 +4625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -7796,7 +7798,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
sensitivity results now aggregate into single spreadsheet
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_var.xlsx
+++ b/data/steel/steel_simplified_var.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56F615F-3FFD-C44F-9322-3A945A349B80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="598" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" tabRatio="598" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="17" r:id="rId1"/>
@@ -33,7 +32,7 @@
     <sheet name="CO2 Storage" sheetId="13" r:id="rId18"/>
     <sheet name="Ref" sheetId="7" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,12 +48,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
+    <comment ref="M5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,12 +117,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -152,12 +151,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -264,12 +263,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
+    <comment ref="K8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,12 +306,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1000-000001000000}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -997,7 +996,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1484,8 +1483,8 @@
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1763,28 +1762,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="20.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -1821,7 +1820,7 @@
       <c r="E2" s="55"/>
       <c r="F2" s="55"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -1833,7 +1832,7 @@
       <c r="E3" s="55"/>
       <c r="F3" s="55"/>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
@@ -1853,7 +1852,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>151</v>
       </c>
@@ -1898,7 +1897,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="69" t="s">
         <v>154</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -1966,7 +1965,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="69" t="s">
         <v>155</v>
       </c>
@@ -1989,17 +1988,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
       <c r="B11" s="57">
-        <f>1/1.2852</f>
-        <v>0.77808901338313108</v>
+        <v>0</v>
       </c>
       <c r="C11" s="57">
-        <f>35*Ref!B18</f>
-        <v>0.126</v>
+        <v>0</v>
       </c>
       <c r="D11" s="42" t="s">
         <v>94</v>
@@ -2011,17 +2008,17 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
       <c r="B12" s="22">
         <f>B11</f>
-        <v>0.77808901338313108</v>
+        <v>0</v>
       </c>
       <c r="C12" s="22">
         <f>C11</f>
-        <v>0.126</v>
+        <v>0</v>
       </c>
       <c r="D12" s="21" t="str">
         <f>D11</f>
@@ -2034,17 +2031,17 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
       <c r="B13" s="29">
         <f t="shared" ref="B13" si="1">B12</f>
-        <v>0.77808901338313108</v>
+        <v>0</v>
       </c>
       <c r="C13" s="29">
         <f t="shared" ref="C13" si="2">C12</f>
-        <v>0.126</v>
+        <v>0</v>
       </c>
       <c r="D13" s="30" t="str">
         <f>D11</f>
@@ -2057,7 +2054,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -2066,7 +2063,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
     </row>
-    <row r="30" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -2082,25 +2079,26 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
-    <col min="2" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2144,7 +2142,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2179,12 +2177,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -2229,7 +2227,7 @@
         <v>0.73399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -2277,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -2323,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>176</v>
       </c>
@@ -2378,7 +2376,7 @@
         <v>0.73399999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>141</v>
       </c>
@@ -2425,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -2481,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>143</v>
       </c>
@@ -2537,7 +2535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>144</v>
       </c>
@@ -2584,7 +2582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -2640,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>146</v>
       </c>
@@ -2704,22 +2702,22 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="21" customWidth="1"/>
     <col min="2" max="2" width="15" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -2739,7 +2737,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -2750,12 +2748,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -2763,7 +2761,7 @@
       <c r="C4" s="45"/>
       <c r="D4" s="45"/>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -2786,7 +2784,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -2811,7 +2809,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -2836,7 +2834,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -2859,7 +2857,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -2884,7 +2882,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -2909,7 +2907,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -2932,7 +2930,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -2957,7 +2955,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -2982,7 +2980,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -3005,7 +3003,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -3030,7 +3028,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -3055,7 +3053,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -3078,7 +3076,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -3103,7 +3101,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -3134,26 +3132,26 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="21" customWidth="1"/>
     <col min="2" max="2" width="15" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.1640625" style="20"/>
+    <col min="6" max="6" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3167,7 +3165,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -3175,12 +3173,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -3192,7 +3190,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -3205,7 +3203,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -3218,7 +3216,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="45" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="38" t="s">
         <v>176</v>
       </c>
@@ -3231,7 +3229,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>150</v>
       </c>
@@ -3244,7 +3242,7 @@
       </c>
       <c r="D8" s="98"/>
     </row>
-    <row r="9" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>151</v>
       </c>
@@ -3257,7 +3255,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>154</v>
       </c>
@@ -3270,7 +3268,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>119</v>
       </c>
@@ -3283,7 +3281,7 @@
       </c>
       <c r="D11" s="98"/>
     </row>
-    <row r="12" spans="1:4" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>152</v>
       </c>
@@ -3297,7 +3295,7 @@
       </c>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:4" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>155</v>
       </c>
@@ -3311,7 +3309,7 @@
       </c>
       <c r="D13" s="45"/>
     </row>
-    <row r="14" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>120</v>
       </c>
@@ -3324,7 +3322,7 @@
       </c>
       <c r="D14" s="20"/>
     </row>
-    <row r="15" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>153</v>
       </c>
@@ -3338,7 +3336,7 @@
       </c>
       <c r="D15" s="20"/>
     </row>
-    <row r="16" spans="1:4" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="63" t="s">
         <v>156</v>
       </c>
@@ -3352,7 +3350,7 @@
       </c>
       <c r="D16" s="45"/>
     </row>
-    <row r="17" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>141</v>
       </c>
@@ -3365,7 +3363,7 @@
       </c>
       <c r="D17" s="20"/>
     </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>142</v>
       </c>
@@ -3379,7 +3377,7 @@
       </c>
       <c r="D18" s="20"/>
     </row>
-    <row r="19" spans="1:4" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>143</v>
       </c>
@@ -3393,7 +3391,7 @@
       </c>
       <c r="D19" s="45"/>
     </row>
-    <row r="20" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>144</v>
       </c>
@@ -3406,7 +3404,7 @@
       </c>
       <c r="D20" s="20"/>
     </row>
-    <row r="21" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>145</v>
       </c>
@@ -3420,7 +3418,7 @@
       </c>
       <c r="D21" s="20"/>
     </row>
-    <row r="22" spans="1:4" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
         <v>146</v>
       </c>
@@ -3434,58 +3432,58 @@
       </c>
       <c r="D22" s="45"/>
     </row>
-    <row r="23" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
     </row>
-    <row r="25" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
     </row>
-    <row r="26" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
     </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
     </row>
-    <row r="28" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
     </row>
-    <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
     </row>
-    <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
     </row>
-    <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
     </row>
-    <row r="32" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
     </row>
-    <row r="36" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -3498,28 +3496,28 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="20" customWidth="1"/>
     <col min="5" max="5" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.1640625" style="20"/>
+    <col min="10" max="16384" width="10.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3543,7 +3541,7 @@
       <c r="I1" s="42"/>
       <c r="J1" s="42"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -3555,12 +3553,12 @@
       </c>
       <c r="G2" s="99"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -3576,7 +3574,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -3592,7 +3590,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -3608,7 +3606,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="45" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>176</v>
       </c>
@@ -3624,7 +3622,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>150</v>
       </c>
@@ -3638,7 +3636,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>151</v>
       </c>
@@ -3654,7 +3652,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>154</v>
       </c>
@@ -3670,7 +3668,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>119</v>
       </c>
@@ -3690,7 +3688,7 @@
       <c r="I11" s="82"/>
       <c r="J11" s="82"/>
     </row>
-    <row r="12" spans="1:10" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>152</v>
       </c>
@@ -3713,7 +3711,7 @@
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
     </row>
-    <row r="13" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>155</v>
       </c>
@@ -3736,7 +3734,7 @@
       <c r="I13" s="45"/>
       <c r="J13" s="45"/>
     </row>
-    <row r="14" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>120</v>
       </c>
@@ -3756,7 +3754,7 @@
       <c r="I14" s="82"/>
       <c r="J14" s="82"/>
     </row>
-    <row r="15" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>153</v>
       </c>
@@ -3779,7 +3777,7 @@
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="1:10" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="63" t="s">
         <v>156</v>
       </c>
@@ -3802,7 +3800,7 @@
       <c r="I16" s="45"/>
       <c r="J16" s="45"/>
     </row>
-    <row r="17" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>141</v>
       </c>
@@ -3822,7 +3820,7 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>142</v>
       </c>
@@ -3845,7 +3843,7 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>143</v>
       </c>
@@ -3868,7 +3866,7 @@
       <c r="I19" s="45"/>
       <c r="J19" s="45"/>
     </row>
-    <row r="20" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>144</v>
       </c>
@@ -3888,7 +3886,7 @@
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>145</v>
       </c>
@@ -3911,7 +3909,7 @@
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="22" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
         <v>146</v>
       </c>
@@ -3934,7 +3932,7 @@
       <c r="I22" s="45"/>
       <c r="J22" s="45"/>
     </row>
-    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
@@ -3945,7 +3943,7 @@
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -3957,7 +3955,7 @@
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
@@ -3968,7 +3966,7 @@
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
@@ -3979,7 +3977,7 @@
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
@@ -3990,7 +3988,7 @@
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -4002,7 +4000,7 @@
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
@@ -4013,7 +4011,7 @@
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
@@ -4024,7 +4022,7 @@
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
     </row>
-    <row r="31" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
@@ -4035,7 +4033,7 @@
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
     </row>
-    <row r="32" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -4047,8 +4045,8 @@
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -4060,7 +4058,7 @@
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
     </row>
-    <row r="40" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -4072,8 +4070,8 @@
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
     </row>
-    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
@@ -4092,27 +4090,27 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="15.83203125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="54" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="20" customWidth="1"/>
+    <col min="5" max="7" width="15.85546875" style="20" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="54" customWidth="1"/>
     <col min="9" max="9" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="21"/>
+    <col min="10" max="10" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -4141,7 +4139,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -4155,12 +4153,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -4174,7 +4172,7 @@
       <c r="I4" s="45"/>
       <c r="J4" s="45"/>
     </row>
-    <row r="5" spans="1:10" s="42" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="42" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -4199,7 +4197,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -4229,7 +4227,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
     </row>
-    <row r="7" spans="1:10" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -4256,7 +4254,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -4282,7 +4280,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -4312,7 +4310,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -4342,7 +4340,7 @@
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -4367,7 +4365,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -4394,7 +4392,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -4423,7 +4421,7 @@
       <c r="I13" s="45"/>
       <c r="J13" s="45"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -4450,7 +4448,7 @@
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -4478,7 +4476,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -4507,7 +4505,7 @@
       <c r="I16" s="45"/>
       <c r="J16" s="45"/>
     </row>
-    <row r="17" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -4533,7 +4531,7 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -4561,7 +4559,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -4590,7 +4588,7 @@
       <c r="I19" s="45"/>
       <c r="J19" s="45"/>
     </row>
-    <row r="21" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -4602,7 +4600,7 @@
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="25" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -4614,7 +4612,7 @@
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4622,7 +4620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4632,16 +4630,16 @@
       <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="21" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" style="21"/>
-    <col min="6" max="6" width="8.83203125" style="96"/>
-    <col min="7" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="26.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="21" customWidth="1"/>
+    <col min="3" max="5" width="8.85546875" style="21"/>
+    <col min="6" max="6" width="8.85546875" style="96"/>
+    <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -4664,7 +4662,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -4685,7 +4683,7 @@
       </c>
       <c r="G2" s="106"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
@@ -4700,7 +4698,7 @@
       <c r="F3" s="115"/>
       <c r="G3" s="106"/>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -4721,7 +4719,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -4745,7 +4743,7 @@
       </c>
       <c r="G5" s="105"/>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -4770,7 +4768,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -4795,7 +4793,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>119</v>
       </c>
@@ -4817,7 +4815,7 @@
       </c>
       <c r="G8" s="108"/>
     </row>
-    <row r="9" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -4843,7 +4841,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -4868,7 +4866,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -4892,7 +4890,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -4917,7 +4915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -4943,7 +4941,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -4969,7 +4967,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -4994,7 +4992,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -5019,7 +5017,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -5043,7 +5041,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -5071,7 +5069,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -5099,7 +5097,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -5108,7 +5106,7 @@
       <c r="F21" s="96"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5117,7 +5115,7 @@
       <c r="F25" s="96"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -5126,7 +5124,7 @@
       <c r="F33" s="96"/>
       <c r="G33" s="21"/>
     </row>
-    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -5142,7 +5140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF35312-EC46-AD4F-8A04-B8DD50E61991}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5152,16 +5150,16 @@
       <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="21" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" style="21"/>
-    <col min="6" max="6" width="8.83203125" style="96"/>
-    <col min="7" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="26.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="21" customWidth="1"/>
+    <col min="3" max="5" width="8.85546875" style="21"/>
+    <col min="6" max="6" width="8.85546875" style="96"/>
+    <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -5184,7 +5182,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -5205,7 +5203,7 @@
       </c>
       <c r="G2" s="106"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
@@ -5220,7 +5218,7 @@
       <c r="F3" s="115"/>
       <c r="G3" s="106"/>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -5239,7 +5237,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="111"/>
     </row>
-    <row r="5" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -5263,7 +5261,7 @@
       </c>
       <c r="G5" s="105"/>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -5288,7 +5286,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -5313,7 +5311,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>119</v>
       </c>
@@ -5337,7 +5335,7 @@
       </c>
       <c r="G8" s="108"/>
     </row>
-    <row r="9" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -5363,7 +5361,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -5388,7 +5386,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -5411,7 +5409,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -5436,7 +5434,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -5462,7 +5460,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -5486,7 +5484,7 @@
       </c>
       <c r="G14" s="105"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -5511,7 +5509,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -5536,7 +5534,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -5560,7 +5558,7 @@
       </c>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -5585,7 +5583,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -5611,7 +5609,7 @@
       </c>
       <c r="G19" s="21"/>
     </row>
-    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -5620,7 +5618,7 @@
       <c r="F21" s="96"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5629,7 +5627,7 @@
       <c r="F25" s="96"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -5638,7 +5636,7 @@
       <c r="F33" s="96"/>
       <c r="G33" s="21"/>
     </row>
-    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -5654,16 +5652,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8A1966-069F-314F-BE37-F818F2948AEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -5674,7 +5672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -5685,7 +5683,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
@@ -5694,7 +5692,7 @@
       </c>
       <c r="C3" s="106"/>
     </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -5705,7 +5703,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -5717,7 +5715,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -5730,7 +5728,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -5743,7 +5741,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>119</v>
       </c>
@@ -5755,7 +5753,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -5768,7 +5766,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -5781,7 +5779,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -5793,7 +5791,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -5806,7 +5804,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -5819,7 +5817,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -5831,7 +5829,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -5844,7 +5842,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -5857,7 +5855,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -5869,7 +5867,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -5882,7 +5880,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -5901,20 +5899,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="21" customWidth="1"/>
-    <col min="2" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="19.140625" style="21" customWidth="1"/>
+    <col min="2" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -5931,7 +5929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -5945,12 +5943,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -5968,7 +5966,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -5986,7 +5984,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -6007,7 +6005,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -6028,7 +6026,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -6047,7 +6045,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -6068,7 +6066,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="69" t="s">
         <v>155</v>
       </c>
@@ -6088,7 +6086,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -6107,7 +6105,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -6128,7 +6126,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -6149,7 +6147,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -6168,7 +6166,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -6189,7 +6187,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -6210,7 +6208,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -6228,7 +6226,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -6249,7 +6247,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="70" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -6270,22 +6268,22 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
     </row>
-    <row r="27" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
     </row>
-    <row r="31" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
     </row>
-    <row r="35" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -6296,33 +6294,33 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>29</v>
@@ -6331,7 +6329,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>31</v>
       </c>
@@ -6343,7 +6341,7 @@
         <v>5.3537967341839917E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
@@ -6355,7 +6353,7 @@
         <v>7.1573391630231102E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>33</v>
       </c>
@@ -6367,7 +6365,7 @@
         <v>1.2496698492013921E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>34</v>
       </c>
@@ -6379,7 +6377,7 @@
         <v>1.963482644775587E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>35</v>
       </c>
@@ -6391,7 +6389,7 @@
         <v>8.9938431337556905E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>36</v>
       </c>
@@ -6403,7 +6401,7 @@
         <v>8.0375122691175155E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
@@ -6416,7 +6414,7 @@
         <v>4.1190030040748338E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
@@ -6428,7 +6426,7 @@
         <v>1.2498170786115822E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>39</v>
       </c>
@@ -6440,31 +6438,31 @@
         <v>1.4276255911483892E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="16"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>42</v>
       </c>
@@ -6473,7 +6471,7 @@
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>43</v>
       </c>
@@ -6483,7 +6481,7 @@
       </c>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>44</v>
       </c>
@@ -6493,7 +6491,7 @@
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>71</v>
       </c>
@@ -6502,7 +6500,7 @@
         <v>1.163</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>73</v>
       </c>
@@ -6518,27 +6516,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.83203125" style="81" customWidth="1"/>
-    <col min="6" max="6" width="63.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="19.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="81" customWidth="1"/>
+    <col min="6" max="6" width="63.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -6558,7 +6556,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -6569,12 +6567,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
@@ -6587,7 +6585,7 @@
       <c r="D4" s="37"/>
       <c r="E4" s="37"/>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -6601,7 +6599,7 @@
       <c r="D5" s="59"/>
       <c r="E5" s="59"/>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -6614,7 +6612,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -6629,7 +6627,7 @@
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
     </row>
-    <row r="8" spans="1:6" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -6644,7 +6642,7 @@
       <c r="E8" s="81"/>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -6657,7 +6655,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="69" t="s">
         <v>155</v>
       </c>
@@ -6672,47 +6670,46 @@
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
       <c r="B11" s="57">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C11" s="57">
-        <f>30*Ref!$B$18</f>
-        <v>0.108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
       <c r="B12" s="21">
         <f>B11</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C12" s="21">
         <f>C11</f>
-        <v>0.108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
       <c r="B13" s="30">
         <f>B11</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C13" s="30">
         <f>C11</f>
-        <v>0.108</v>
+        <v>0</v>
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="37"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -6724,7 +6721,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -6737,7 +6734,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -6752,7 +6749,7 @@
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -6764,7 +6761,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -6777,7 +6774,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -6793,7 +6790,7 @@
       <c r="E19" s="37"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A26:F49">
+  <sortState ref="A26:F49">
     <sortCondition ref="A26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6802,29 +6799,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="81" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="21" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="20.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="81" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -6853,7 +6850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -6864,13 +6861,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="85"/>
     </row>
-    <row r="4" spans="1:9" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -6895,7 +6892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -6924,7 +6921,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -6954,7 +6951,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -6983,7 +6980,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -7004,7 +7001,7 @@
         <v>113</v>
       </c>
       <c r="G8" s="57">
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="42">
         <f>75*Ref!$B$18</f>
@@ -7012,7 +7009,7 @@
       </c>
       <c r="I8" s="42"/>
     </row>
-    <row r="9" spans="1:9" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -7035,7 +7032,7 @@
       </c>
       <c r="G9" s="21">
         <f>G8</f>
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H9" s="21">
         <f>H8</f>
@@ -7043,7 +7040,7 @@
       </c>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:9" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -7065,14 +7062,14 @@
       </c>
       <c r="G10" s="30">
         <f>G8</f>
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H10" s="30">
         <f>H8</f>
         <v>0.27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -7080,8 +7077,7 @@
         <v>0.72</v>
       </c>
       <c r="C11" s="57">
-        <f>0.72/25.8</f>
-        <v>2.7906976744186046E-2</v>
+        <v>2.6100000000000002E-2</v>
       </c>
       <c r="D11" s="42" t="s">
         <v>118</v>
@@ -7093,21 +7089,20 @@
         <v>113</v>
       </c>
       <c r="G11" s="57">
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H11" s="42">
-        <f>75*Ref!$B$18</f>
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
       <c r="B12" s="89"/>
       <c r="C12" s="28">
         <f>C11</f>
-        <v>2.7906976744186046E-2</v>
+        <v>2.6100000000000002E-2</v>
       </c>
       <c r="D12" s="28" t="str">
         <f>D11</f>
@@ -7123,21 +7118,21 @@
       </c>
       <c r="G12" s="28">
         <f>G11</f>
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="43">
         <f>H11</f>
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
       <c r="B13" s="88"/>
       <c r="C13" s="39">
         <f>C11</f>
-        <v>2.7906976744186046E-2</v>
+        <v>2.6100000000000002E-2</v>
       </c>
       <c r="D13" s="39" t="str">
         <f>D11</f>
@@ -7152,15 +7147,15 @@
       </c>
       <c r="G13" s="39">
         <f>G11</f>
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="44">
         <f>H11</f>
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="I13" s="30"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -7189,7 +7184,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -7218,7 +7213,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -7246,7 +7241,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -7276,7 +7271,7 @@
       </c>
       <c r="I17" s="21"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -7305,7 +7300,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -7333,7 +7328,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="81"/>
       <c r="C21" s="21"/>
@@ -7344,7 +7339,7 @@
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="33" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="81"/>
       <c r="C33" s="21"/>
@@ -7355,7 +7350,7 @@
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
     </row>
-    <row r="37" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="81"/>
       <c r="C37" s="21"/>
@@ -7373,29 +7368,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="22.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7421,7 +7416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -7438,12 +7433,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -7468,7 +7463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -7494,7 +7489,7 @@
       </c>
       <c r="H5" s="42"/>
     </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -7522,7 +7517,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -7550,7 +7545,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -7575,7 +7570,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -7603,7 +7598,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -7631,7 +7626,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -7648,16 +7643,14 @@
         <v>113</v>
       </c>
       <c r="F11" s="57">
-        <f>0.01+(0.1165*(56/100))</f>
-        <v>7.5240000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G11" s="57">
-        <f>32*Ref!$B$18</f>
-        <v>0.1152</v>
+        <v>0</v>
       </c>
       <c r="H11" s="42"/>
     </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -7678,14 +7671,14 @@
       </c>
       <c r="F12" s="22">
         <f>F11</f>
-        <v>7.5240000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="22">
         <f>G11</f>
-        <v>0.1152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
         <v>156</v>
       </c>
@@ -7706,14 +7699,14 @@
       </c>
       <c r="F13" s="22">
         <f>F11</f>
-        <v>7.5240000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="22">
         <f>G11</f>
-        <v>0.1152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -7723,7 +7716,7 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="31" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -7733,7 +7726,7 @@
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
     </row>
-    <row r="35" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -7743,7 +7736,7 @@
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
     </row>
-    <row r="39" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -7753,7 +7746,7 @@
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
     </row>
-    <row r="47" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -7763,8 +7756,8 @@
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -7774,7 +7767,7 @@
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
     </row>
-    <row r="63" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
@@ -7791,35 +7784,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" style="21" customWidth="1"/>
-    <col min="2" max="4" width="11.5" style="21"/>
+    <col min="2" max="4" width="11.42578125" style="21"/>
     <col min="5" max="6" width="0" style="129" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="21"/>
-    <col min="8" max="8" width="11.5" style="27"/>
-    <col min="9" max="9" width="9.83203125" style="21" customWidth="1"/>
-    <col min="10" max="13" width="11.5" style="21"/>
-    <col min="14" max="14" width="20.6640625" style="21" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="21" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="21"/>
-    <col min="17" max="17" width="12.5" style="81" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="21"/>
+    <col min="8" max="8" width="11.42578125" style="27"/>
+    <col min="9" max="9" width="9.85546875" style="21" customWidth="1"/>
+    <col min="10" max="13" width="11.42578125" style="21"/>
+    <col min="14" max="14" width="20.7109375" style="21" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="21" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="21"/>
+    <col min="17" max="17" width="12.42578125" style="81" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="0" style="81" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5" style="55"/>
-    <col min="20" max="16384" width="11.5" style="21"/>
+    <col min="19" max="19" width="11.42578125" style="55"/>
+    <col min="20" max="16384" width="11.42578125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7881,7 +7874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -7920,7 +7913,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -7930,7 +7923,7 @@
       <c r="E3" s="125"/>
       <c r="F3" s="125"/>
     </row>
-    <row r="4" spans="1:20" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -7981,7 +7974,7 @@
       <c r="R4" s="37"/>
       <c r="S4" s="84"/>
     </row>
-    <row r="5" spans="1:20" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -8041,7 +8034,7 @@
         <v>13.926959999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -8106,7 +8099,7 @@
         <v>13.926959999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -8171,7 +8164,7 @@
         <v>13.926959999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
         <v>119</v>
       </c>
@@ -8230,7 +8223,7 @@
       </c>
       <c r="T8" s="26"/>
     </row>
-    <row r="9" spans="1:20" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -8294,7 +8287,7 @@
         <v>11.0562</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -8363,7 +8356,7 @@
         <v>11.0562</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -8374,8 +8367,8 @@
         <v>1.7</v>
       </c>
       <c r="D11" s="57">
-        <f>(1.1+18*(56/100)+9*(0.477/0.44))/145</f>
-        <v>0.14439184952978057</v>
+        <f>(1.1+18*(56/100)+9*(0.477/0.44)*(56/100))/145</f>
+        <v>0.11478495297805644</v>
       </c>
       <c r="E11" s="127">
         <v>8.9999999999999993E-3</v>
@@ -8388,8 +8381,8 @@
         <v>0.3</v>
       </c>
       <c r="H11" s="35">
-        <f>3400/(8000/365)/145</f>
-        <v>1.0698275862068964</v>
+        <f>3400/24/145</f>
+        <v>0.97701149425287348</v>
       </c>
       <c r="I11" s="34">
         <v>0</v>
@@ -8428,7 +8421,7 @@
       </c>
       <c r="T11" s="42"/>
     </row>
-    <row r="12" spans="1:20" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -8442,7 +8435,7 @@
       </c>
       <c r="D12" s="56">
         <f>D11</f>
-        <v>0.14439184952978057</v>
+        <v>0.11478495297805644</v>
       </c>
       <c r="E12" s="127">
         <v>8.9999999999999993E-3</v>
@@ -8457,7 +8450,7 @@
       </c>
       <c r="H12" s="56">
         <f t="shared" si="6"/>
-        <v>1.0698275862068964</v>
+        <v>0.97701149425287348</v>
       </c>
       <c r="I12" s="26">
         <f>I11</f>
@@ -8496,7 +8489,7 @@
         <v>15.738</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
         <v>156</v>
       </c>
@@ -8510,7 +8503,7 @@
       </c>
       <c r="D13" s="22">
         <f>D11</f>
-        <v>0.14439184952978057</v>
+        <v>0.11478495297805644</v>
       </c>
       <c r="E13" s="127">
         <v>8.9999999999999993E-3</v>
@@ -8525,7 +8518,7 @@
       </c>
       <c r="H13" s="22">
         <f t="shared" si="7"/>
-        <v>1.0698275862068964</v>
+        <v>0.97701149425287348</v>
       </c>
       <c r="I13" s="21">
         <f>I11</f>
@@ -8565,11 +8558,11 @@
       </c>
       <c r="T13" s="21"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H14" s="21"/>
       <c r="S14" s="118"/>
     </row>
-    <row r="17" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -8591,7 +8584,7 @@
       <c r="S17" s="55"/>
       <c r="T17" s="21"/>
     </row>
-    <row r="21" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -8613,7 +8606,7 @@
       <c r="S21" s="55"/>
       <c r="T21" s="21"/>
     </row>
-    <row r="25" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -8635,14 +8628,14 @@
       <c r="S25" s="55"/>
       <c r="T25" s="21"/>
     </row>
-    <row r="29" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E29" s="124"/>
       <c r="F29" s="124"/>
       <c r="Q29" s="116"/>
       <c r="R29" s="116"/>
       <c r="S29" s="64"/>
     </row>
-    <row r="33" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -8664,7 +8657,7 @@
       <c r="S33" s="55"/>
       <c r="T33" s="21"/>
     </row>
-    <row r="34" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -8686,7 +8679,7 @@
       <c r="S34" s="55"/>
       <c r="T34" s="21"/>
     </row>
-    <row r="41" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -8716,7 +8709,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8726,24 +8719,24 @@
       <selection pane="bottomRight" activeCell="F1" sqref="F1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="81" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="81" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="81" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="81" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="21"/>
+    <col min="13" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -8784,7 +8777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -8804,7 +8797,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -8813,7 +8806,7 @@
       </c>
       <c r="C3" s="85"/>
     </row>
-    <row r="4" spans="1:13" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -8850,7 +8843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -8896,7 +8889,7 @@
       </c>
       <c r="M5" s="42"/>
     </row>
-    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -8945,7 +8938,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -8994,7 +8987,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>119</v>
       </c>
@@ -9040,7 +9033,7 @@
       </c>
       <c r="M8" s="42"/>
     </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -9089,7 +9082,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -9138,7 +9131,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -9184,7 +9177,7 @@
       </c>
       <c r="M11" s="21"/>
     </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -9233,7 +9226,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -9282,7 +9275,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="81"/>
@@ -9297,7 +9290,7 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
     </row>
-    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
       <c r="C18" s="81"/>
@@ -9312,7 +9305,7 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="22" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="81"/>
@@ -9327,7 +9320,7 @@
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
     </row>
-    <row r="26" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="81"/>
@@ -9342,7 +9335,7 @@
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
     </row>
-    <row r="30" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="81"/>
@@ -9357,7 +9350,7 @@
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
     </row>
-    <row r="34" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="81"/>
@@ -9372,7 +9365,7 @@
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
     </row>
-    <row r="38" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="81"/>
@@ -9394,27 +9387,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="8" width="8.83203125" style="36"/>
-    <col min="9" max="9" width="9.1640625" style="36"/>
-    <col min="12" max="15" width="8.83203125" style="36"/>
+    <col min="1" max="1" width="21.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="36"/>
+    <col min="9" max="9" width="9.140625" style="36"/>
+    <col min="12" max="15" width="8.85546875" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -9464,7 +9457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9505,12 +9498,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>191</v>
       </c>
@@ -9549,7 +9542,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>199</v>
       </c>
@@ -9587,7 +9580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>197</v>
       </c>
@@ -9631,7 +9624,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>198</v>
       </c>
@@ -9674,7 +9667,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="139" t="s">
         <v>206</v>
       </c>
@@ -9707,7 +9700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="139" t="s">
         <v>207</v>
       </c>
@@ -9740,7 +9733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>3</v>
       </c>
@@ -9800,7 +9793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>150</v>
       </c>
@@ -9846,7 +9839,7 @@
       <c r="N11"/>
       <c r="O11"/>
     </row>
-    <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>151</v>
       </c>
@@ -9892,7 +9885,7 @@
       <c r="N12"/>
       <c r="O12"/>
     </row>
-    <row r="13" spans="1:16" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>154</v>
       </c>
@@ -9933,7 +9926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>119</v>
       </c>
@@ -9979,7 +9972,7 @@
       <c r="N14"/>
       <c r="O14"/>
     </row>
-    <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>152</v>
       </c>
@@ -10025,7 +10018,7 @@
       <c r="N15"/>
       <c r="O15"/>
     </row>
-    <row r="16" spans="1:16" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="63" t="s">
         <v>155</v>
       </c>
@@ -10066,7 +10059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
         <v>120</v>
       </c>
@@ -10112,7 +10105,7 @@
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
         <v>153</v>
       </c>
@@ -10158,7 +10151,7 @@
       <c r="N18"/>
       <c r="O18"/>
     </row>
-    <row r="19" spans="1:15" s="37" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="88" t="s">
         <v>156</v>
       </c>
@@ -10212,24 +10205,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10255,7 +10248,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -10278,19 +10271,19 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="29"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -10318,7 +10311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -10349,7 +10342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>143</v>
       </c>
@@ -10380,7 +10373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>144</v>
       </c>
@@ -10408,7 +10401,7 @@
         <v>0.22842009458374227</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>145</v>
       </c>
@@ -10440,7 +10433,7 @@
         <v>0.22842009458374227</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>146</v>
       </c>
@@ -10479,28 +10472,28 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="21" customWidth="1"/>
     <col min="9" max="9" width="19" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="21"/>
+    <col min="10" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10538,7 +10531,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -10564,7 +10557,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -10572,7 +10565,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -10607,7 +10600,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>147</v>
       </c>
@@ -10644,7 +10637,7 @@
         <v>4.2828767734451677E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>148</v>
       </c>
@@ -10663,7 +10656,7 @@
         <v>natural gas - IPCC</v>
       </c>
       <c r="F6" s="51">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>113</v>
@@ -10682,7 +10675,7 @@
         <v>7.1381279557419458E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>149</v>
       </c>
@@ -10701,7 +10694,7 @@
         <v>natural gas - IPCC</v>
       </c>
       <c r="F7" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>113</v>
@@ -10720,7 +10713,7 @@
         <v>7.1381279557419458E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>141</v>
       </c>
@@ -10761,7 +10754,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>142</v>
       </c>
@@ -10803,7 +10796,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>143</v>
       </c>
@@ -10823,7 +10816,7 @@
         <v>natural gas - IPCC</v>
       </c>
       <c r="F10" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="30" t="s">
         <v>113</v>
@@ -10845,7 +10838,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>144</v>
       </c>
@@ -10884,7 +10877,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>145</v>
       </c>
@@ -10926,7 +10919,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>146</v>
       </c>
@@ -10946,7 +10939,7 @@
         <v>natural gas - IPCC</v>
       </c>
       <c r="F13" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="30" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
no actual change; excel is stupid
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_var.xlsx
+++ b/data/steel/steel_simplified_var.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" tabRatio="598" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" tabRatio="598" firstSheet="13" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="17" r:id="rId1"/>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="215">
   <si>
     <t>scenario</t>
   </si>
@@ -991,6 +991,9 @@
   </si>
   <si>
     <t>from 2013 - TGR scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -6295,10 +6298,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6306,21 +6309,21 @@
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>29</v>
@@ -6329,7 +6332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>31</v>
       </c>
@@ -6341,7 +6344,7 @@
         <v>5.3537967341839917E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
@@ -6353,7 +6356,7 @@
         <v>7.1573391630231102E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>33</v>
       </c>
@@ -6365,7 +6368,7 @@
         <v>1.2496698492013921E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>34</v>
       </c>
@@ -6377,7 +6380,7 @@
         <v>1.963482644775587E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>35</v>
       </c>
@@ -6389,7 +6392,7 @@
         <v>8.9938431337556905E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>36</v>
       </c>
@@ -6401,7 +6404,7 @@
         <v>8.0375122691175155E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
@@ -6414,7 +6417,7 @@
         <v>4.1190030040748338E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
@@ -6426,7 +6429,7 @@
         <v>1.2498170786115822E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>39</v>
       </c>
@@ -6438,31 +6441,32 @@
         <v>1.4276255911483892E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="16"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H16" s="122"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>42</v>
       </c>
@@ -6471,7 +6475,7 @@
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>43</v>
       </c>
@@ -6480,8 +6484,10 @@
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="23"/>
+      <c r="E18" s="122"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>44</v>
       </c>
@@ -6491,7 +6497,7 @@
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>71</v>
       </c>
@@ -6499,14 +6505,20 @@
         <f>1.163</f>
         <v>1.163</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="122"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>73</v>
       </c>
       <c r="B21" s="22">
         <f>2000/2204.62</f>
         <v>0.90718581887127947</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -7788,7 +7800,7 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
@@ -10475,8 +10487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
heat recovery is excluded for BFF and TGR now
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_var.xlsx
+++ b/data/steel/steel_simplified_var.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\steel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E45BD73-511C-EC49-8317-DB8201295DE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" tabRatio="598" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="598" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="17" r:id="rId1"/>
@@ -32,7 +33,7 @@
     <sheet name="CO2 Storage" sheetId="13" r:id="rId18"/>
     <sheet name="Ref" sheetId="7" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,12 +49,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0">
+    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -117,12 +118,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -151,12 +152,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -190,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -224,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -263,12 +264,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="K8" authorId="0" shapeId="0">
+    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -306,12 +307,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -999,7 +1000,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1486,8 +1487,8 @@
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1765,7 +1766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1775,18 +1776,18 @@
       <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="20.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +1810,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -1823,7 +1824,7 @@
       <c r="E2" s="55"/>
       <c r="F2" s="55"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -1835,7 +1836,7 @@
       <c r="E3" s="55"/>
       <c r="F3" s="55"/>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -1877,7 +1878,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="60" t="s">
         <v>151</v>
       </c>
@@ -1900,7 +1901,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
         <v>154</v>
       </c>
@@ -1923,7 +1924,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -1945,7 +1946,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -1968,7 +1969,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="69" t="s">
         <v>155</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -2011,7 +2012,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -2034,7 +2035,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -2057,7 +2058,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -2066,7 +2067,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
     </row>
-    <row r="30" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="26"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -2082,26 +2083,26 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2180,12 +2181,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -2230,7 +2231,7 @@
         <v>0.73399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -2324,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>176</v>
       </c>
@@ -2379,7 +2380,7 @@
         <v>0.73399999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>141</v>
       </c>
@@ -2426,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -2482,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>143</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>144</v>
       </c>
@@ -2585,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -2641,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>146</v>
       </c>
@@ -2705,22 +2706,22 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" style="21" customWidth="1"/>
     <col min="2" max="2" width="15" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -2751,12 +2752,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -2764,7 +2765,7 @@
       <c r="C4" s="45"/>
       <c r="D4" s="45"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -2787,7 +2788,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -2812,7 +2813,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -2860,7 +2861,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -2910,7 +2911,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -2933,7 +2934,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -2958,7 +2959,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -2983,7 +2984,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -3006,7 +3007,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -3031,7 +3032,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -3056,7 +3057,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -3104,7 +3105,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -3135,26 +3136,26 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" style="21" customWidth="1"/>
     <col min="2" max="2" width="15" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.140625" style="20"/>
+    <col min="6" max="6" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.1640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3168,7 +3169,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -3176,12 +3177,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -3193,7 +3194,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -3206,7 +3207,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -3219,7 +3220,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="45" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>176</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>150</v>
       </c>
@@ -3245,7 +3246,7 @@
       </c>
       <c r="D8" s="98"/>
     </row>
-    <row r="9" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>151</v>
       </c>
@@ -3258,7 +3259,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>154</v>
       </c>
@@ -3271,7 +3272,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
         <v>119</v>
       </c>
@@ -3284,7 +3285,7 @@
       </c>
       <c r="D11" s="98"/>
     </row>
-    <row r="12" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="60" t="s">
         <v>152</v>
       </c>
@@ -3298,7 +3299,7 @@
       </c>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>155</v>
       </c>
@@ -3312,7 +3313,7 @@
       </c>
       <c r="D13" s="45"/>
     </row>
-    <row r="14" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="62" t="s">
         <v>120</v>
       </c>
@@ -3325,7 +3326,7 @@
       </c>
       <c r="D14" s="20"/>
     </row>
-    <row r="15" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="53" t="s">
         <v>153</v>
       </c>
@@ -3339,7 +3340,7 @@
       </c>
       <c r="D15" s="20"/>
     </row>
-    <row r="16" spans="1:4" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
         <v>156</v>
       </c>
@@ -3353,7 +3354,7 @@
       </c>
       <c r="D16" s="45"/>
     </row>
-    <row r="17" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>141</v>
       </c>
@@ -3366,7 +3367,7 @@
       </c>
       <c r="D17" s="20"/>
     </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>142</v>
       </c>
@@ -3380,7 +3381,7 @@
       </c>
       <c r="D18" s="20"/>
     </row>
-    <row r="19" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>143</v>
       </c>
@@ -3394,7 +3395,7 @@
       </c>
       <c r="D19" s="45"/>
     </row>
-    <row r="20" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>144</v>
       </c>
@@ -3407,7 +3408,7 @@
       </c>
       <c r="D20" s="20"/>
     </row>
-    <row r="21" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
         <v>145</v>
       </c>
@@ -3421,7 +3422,7 @@
       </c>
       <c r="D21" s="20"/>
     </row>
-    <row r="22" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>146</v>
       </c>
@@ -3435,58 +3436,58 @@
       </c>
       <c r="D22" s="45"/>
     </row>
-    <row r="23" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
     </row>
-    <row r="25" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
     </row>
-    <row r="26" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
     </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
     </row>
-    <row r="28" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
     </row>
-    <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
     </row>
-    <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
     </row>
-    <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
     </row>
-    <row r="32" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
     </row>
-    <row r="36" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="21"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -3499,28 +3500,28 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="20" customWidth="1"/>
     <col min="5" max="5" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.140625" style="20"/>
+    <col min="10" max="16384" width="10.1640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3544,7 +3545,7 @@
       <c r="I1" s="42"/>
       <c r="J1" s="42"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -3556,12 +3557,12 @@
       </c>
       <c r="G2" s="99"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -3593,7 +3594,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -3609,7 +3610,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" s="45" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>176</v>
       </c>
@@ -3625,7 +3626,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>150</v>
       </c>
@@ -3639,7 +3640,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>151</v>
       </c>
@@ -3655,7 +3656,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>154</v>
       </c>
@@ -3671,7 +3672,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
         <v>119</v>
       </c>
@@ -3691,7 +3692,7 @@
       <c r="I11" s="82"/>
       <c r="J11" s="82"/>
     </row>
-    <row r="12" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="60" t="s">
         <v>152</v>
       </c>
@@ -3714,7 +3715,7 @@
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
     </row>
-    <row r="13" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>155</v>
       </c>
@@ -3737,7 +3738,7 @@
       <c r="I13" s="45"/>
       <c r="J13" s="45"/>
     </row>
-    <row r="14" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="62" t="s">
         <v>120</v>
       </c>
@@ -3757,7 +3758,7 @@
       <c r="I14" s="82"/>
       <c r="J14" s="82"/>
     </row>
-    <row r="15" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="53" t="s">
         <v>153</v>
       </c>
@@ -3780,7 +3781,7 @@
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="1:10" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
         <v>156</v>
       </c>
@@ -3803,7 +3804,7 @@
       <c r="I16" s="45"/>
       <c r="J16" s="45"/>
     </row>
-    <row r="17" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>141</v>
       </c>
@@ -3823,7 +3824,7 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>142</v>
       </c>
@@ -3846,7 +3847,7 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>143</v>
       </c>
@@ -3869,7 +3870,7 @@
       <c r="I19" s="45"/>
       <c r="J19" s="45"/>
     </row>
-    <row r="20" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>144</v>
       </c>
@@ -3889,7 +3890,7 @@
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
         <v>145</v>
       </c>
@@ -3912,7 +3913,7 @@
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="22" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>146</v>
       </c>
@@ -3935,7 +3936,7 @@
       <c r="I22" s="45"/>
       <c r="J22" s="45"/>
     </row>
-    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
@@ -3946,7 +3947,7 @@
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -3958,7 +3959,7 @@
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
@@ -3969,7 +3970,7 @@
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
@@ -3980,7 +3981,7 @@
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
@@ -3991,7 +3992,7 @@
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -4003,7 +4004,7 @@
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
@@ -4014,7 +4015,7 @@
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
@@ -4025,7 +4026,7 @@
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
     </row>
-    <row r="31" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
@@ -4036,7 +4037,7 @@
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
     </row>
-    <row r="32" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -4048,8 +4049,8 @@
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="21"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -4061,7 +4062,7 @@
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
     </row>
-    <row r="40" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="21"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -4073,8 +4074,8 @@
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
     </row>
-    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="21"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
@@ -4093,27 +4094,27 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="20" customWidth="1"/>
-    <col min="5" max="7" width="15.85546875" style="20" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="54" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="20" customWidth="1"/>
+    <col min="5" max="7" width="15.83203125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" style="54" customWidth="1"/>
     <col min="9" max="9" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="21"/>
+    <col min="10" max="10" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -4142,7 +4143,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -4156,12 +4157,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -4175,7 +4176,7 @@
       <c r="I4" s="45"/>
       <c r="J4" s="45"/>
     </row>
-    <row r="5" spans="1:10" s="42" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="42" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -4183,8 +4184,7 @@
         <v>0.9</v>
       </c>
       <c r="C5" s="47">
-        <f>1-(0.5736/(0.5736+2.9763+0.6597))</f>
-        <v>0.86374002280501716</v>
+        <v>0</v>
       </c>
       <c r="D5" s="42" t="s">
         <v>95</v>
@@ -4200,7 +4200,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="C6" s="10">
         <f t="shared" ref="C6" si="0">C$5</f>
-        <v>0.86374002280501716</v>
+        <v>0</v>
       </c>
       <c r="D6" s="21" t="str">
         <f>D5</f>
@@ -4230,7 +4230,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
     </row>
-    <row r="7" spans="1:10" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -4240,7 +4240,7 @@
       </c>
       <c r="C7" s="46">
         <f t="shared" si="1"/>
-        <v>0.86374002280501716</v>
+        <v>0</v>
       </c>
       <c r="D7" s="21" t="str">
         <f>D6</f>
@@ -4257,7 +4257,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -4265,8 +4265,7 @@
         <v>0.9</v>
       </c>
       <c r="C8" s="41">
-        <f>1-(0.6535/(0.6535+0.8435+0.6597))</f>
-        <v>0.69699077294014</v>
+        <v>0</v>
       </c>
       <c r="D8" s="42" t="s">
         <v>95</v>
@@ -4283,7 +4282,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -4293,7 +4292,7 @@
       </c>
       <c r="C9" s="10">
         <f>C8</f>
-        <v>0.69699077294014</v>
+        <v>0</v>
       </c>
       <c r="D9" s="21" t="str">
         <f>D8</f>
@@ -4313,7 +4312,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -4323,7 +4322,7 @@
       </c>
       <c r="C10" s="46">
         <f>C8</f>
-        <v>0.69699077294014</v>
+        <v>0</v>
       </c>
       <c r="D10" s="21" t="str">
         <f>D9</f>
@@ -4343,7 +4342,7 @@
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -4368,7 +4367,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -4395,7 +4394,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -4424,7 +4423,7 @@
       <c r="I13" s="45"/>
       <c r="J13" s="45"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -4451,7 +4450,7 @@
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -4479,7 +4478,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -4508,7 +4507,7 @@
       <c r="I16" s="45"/>
       <c r="J16" s="45"/>
     </row>
-    <row r="17" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -4534,7 +4533,7 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -4562,7 +4561,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -4591,7 +4590,7 @@
       <c r="I19" s="45"/>
       <c r="J19" s="45"/>
     </row>
-    <row r="21" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -4603,7 +4602,7 @@
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="25" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -4615,7 +4614,7 @@
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4623,7 +4622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4633,16 +4632,16 @@
       <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="21" customWidth="1"/>
-    <col min="3" max="5" width="8.85546875" style="21"/>
-    <col min="6" max="6" width="8.85546875" style="96"/>
-    <col min="7" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="26.5" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="21" customWidth="1"/>
+    <col min="3" max="5" width="8.83203125" style="21"/>
+    <col min="6" max="6" width="8.83203125" style="96"/>
+    <col min="7" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -4665,7 +4664,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -4686,7 +4685,7 @@
       </c>
       <c r="G2" s="106"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
@@ -4701,7 +4700,7 @@
       <c r="F3" s="115"/>
       <c r="G3" s="106"/>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -4722,7 +4721,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -4746,7 +4745,7 @@
       </c>
       <c r="G5" s="105"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -4796,7 +4795,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="80" t="s">
         <v>119</v>
       </c>
@@ -4818,7 +4817,7 @@
       </c>
       <c r="G8" s="108"/>
     </row>
-    <row r="9" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -4844,7 +4843,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -4869,7 +4868,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -4893,7 +4892,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -4918,7 +4917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -4944,7 +4943,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -4970,7 +4969,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -4995,7 +4994,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -5020,7 +5019,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -5044,7 +5043,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -5072,7 +5071,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -5100,7 +5099,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -5109,7 +5108,7 @@
       <c r="F21" s="96"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5118,7 +5117,7 @@
       <c r="F25" s="96"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -5127,7 +5126,7 @@
       <c r="F33" s="96"/>
       <c r="G33" s="21"/>
     </row>
-    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -5143,7 +5142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5153,16 +5152,16 @@
       <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="21" customWidth="1"/>
-    <col min="3" max="5" width="8.85546875" style="21"/>
-    <col min="6" max="6" width="8.85546875" style="96"/>
-    <col min="7" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="26.5" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="21" customWidth="1"/>
+    <col min="3" max="5" width="8.83203125" style="21"/>
+    <col min="6" max="6" width="8.83203125" style="96"/>
+    <col min="7" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -5185,7 +5184,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -5206,7 +5205,7 @@
       </c>
       <c r="G2" s="106"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
@@ -5221,7 +5220,7 @@
       <c r="F3" s="115"/>
       <c r="G3" s="106"/>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -5240,7 +5239,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="111"/>
     </row>
-    <row r="5" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -5264,7 +5263,7 @@
       </c>
       <c r="G5" s="105"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -5289,7 +5288,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -5314,7 +5313,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="80" t="s">
         <v>119</v>
       </c>
@@ -5338,7 +5337,7 @@
       </c>
       <c r="G8" s="108"/>
     </row>
-    <row r="9" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -5364,7 +5363,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -5389,7 +5388,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -5412,7 +5411,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -5437,7 +5436,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -5463,7 +5462,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -5487,7 +5486,7 @@
       </c>
       <c r="G14" s="105"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -5512,7 +5511,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -5537,7 +5536,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -5561,7 +5560,7 @@
       </c>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -5586,7 +5585,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -5612,7 +5611,7 @@
       </c>
       <c r="G19" s="21"/>
     </row>
-    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -5621,7 +5620,7 @@
       <c r="F21" s="96"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5630,7 +5629,7 @@
       <c r="F25" s="96"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -5639,7 +5638,7 @@
       <c r="F33" s="96"/>
       <c r="G33" s="21"/>
     </row>
-    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -5655,16 +5654,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -5675,7 +5674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -5686,7 +5685,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
@@ -5695,7 +5694,7 @@
       </c>
       <c r="C3" s="106"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -5706,7 +5705,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -5718,7 +5717,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -5731,7 +5730,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -5744,7 +5743,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="80" t="s">
         <v>119</v>
       </c>
@@ -5756,7 +5755,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -5769,7 +5768,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -5782,7 +5781,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -5794,7 +5793,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -5807,7 +5806,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -5820,7 +5819,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -5832,7 +5831,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -5845,7 +5844,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -5858,7 +5857,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -5870,7 +5869,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -5883,7 +5882,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -5902,20 +5901,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="21" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="19.1640625" style="21" customWidth="1"/>
+    <col min="2" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -5932,7 +5931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -5946,12 +5945,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -5969,7 +5968,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -5987,7 +5986,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -6008,7 +6007,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -6029,7 +6028,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -6048,7 +6047,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -6069,7 +6068,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="69" t="s">
         <v>155</v>
       </c>
@@ -6089,7 +6088,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -6108,7 +6107,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -6129,7 +6128,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -6150,7 +6149,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -6169,7 +6168,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -6190,7 +6189,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -6211,7 +6210,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -6229,7 +6228,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -6250,7 +6249,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="70" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -6271,22 +6270,22 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
     </row>
-    <row r="27" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
     </row>
-    <row r="31" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
     </row>
-    <row r="35" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -6297,33 +6296,33 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>29</v>
@@ -6332,7 +6331,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>31</v>
       </c>
@@ -6344,7 +6343,7 @@
         <v>5.3537967341839917E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
@@ -6356,7 +6355,7 @@
         <v>7.1573391630231102E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>33</v>
       </c>
@@ -6368,7 +6367,7 @@
         <v>1.2496698492013921E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>34</v>
       </c>
@@ -6380,7 +6379,7 @@
         <v>1.963482644775587E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>35</v>
       </c>
@@ -6392,7 +6391,7 @@
         <v>8.9938431337556905E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>36</v>
       </c>
@@ -6404,7 +6403,7 @@
         <v>8.0375122691175155E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
@@ -6417,7 +6416,7 @@
         <v>4.1190030040748338E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
@@ -6429,7 +6428,7 @@
         <v>1.2498170786115822E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>39</v>
       </c>
@@ -6441,24 +6440,24 @@
         <v>1.4276255911483892E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="16" t="s">
         <v>41</v>
@@ -6466,7 +6465,7 @@
       <c r="C16" s="16"/>
       <c r="H16" s="122"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>42</v>
       </c>
@@ -6475,7 +6474,7 @@
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>43</v>
       </c>
@@ -6487,7 +6486,7 @@
       <c r="D18" s="23"/>
       <c r="E18" s="122"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>44</v>
       </c>
@@ -6497,7 +6496,7 @@
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>71</v>
       </c>
@@ -6507,7 +6506,7 @@
       </c>
       <c r="E20" s="122"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>73</v>
       </c>
@@ -6516,7 +6515,7 @@
         <v>0.90718581887127947</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
         <v>214</v>
       </c>
@@ -6528,7 +6527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6538,17 +6537,17 @@
       <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" style="81" customWidth="1"/>
-    <col min="6" max="6" width="63.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="19.5" style="21" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.83203125" style="81" customWidth="1"/>
+    <col min="6" max="6" width="63.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -6568,7 +6567,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -6579,12 +6578,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
@@ -6597,7 +6596,7 @@
       <c r="D4" s="37"/>
       <c r="E4" s="37"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -6611,7 +6610,7 @@
       <c r="D5" s="59"/>
       <c r="E5" s="59"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -6624,7 +6623,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -6639,7 +6638,7 @@
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
     </row>
-    <row r="8" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -6654,7 +6653,7 @@
       <c r="E8" s="81"/>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -6667,7 +6666,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="69" t="s">
         <v>155</v>
       </c>
@@ -6682,7 +6681,7 @@
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -6693,7 +6692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -6706,7 +6705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -6721,7 +6720,7 @@
       <c r="D13" s="37"/>
       <c r="E13" s="37"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -6733,7 +6732,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -6746,7 +6745,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -6761,7 +6760,7 @@
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -6773,7 +6772,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -6786,7 +6785,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -6802,7 +6801,7 @@
       <c r="E19" s="37"/>
     </row>
   </sheetData>
-  <sortState ref="A26:F49">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A26:F49">
     <sortCondition ref="A26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6811,7 +6810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6821,19 +6820,19 @@
       <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="81" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="20.1640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="81" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="21" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -6862,7 +6861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -6873,13 +6872,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="85"/>
     </row>
-    <row r="4" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -6904,7 +6903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -6933,7 +6932,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -6963,7 +6962,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -6992,7 +6991,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -7021,7 +7020,7 @@
       </c>
       <c r="I8" s="42"/>
     </row>
-    <row r="9" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -7052,7 +7051,7 @@
       </c>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -7081,7 +7080,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -7107,7 +7106,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -7137,7 +7136,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -7167,7 +7166,7 @@
       </c>
       <c r="I13" s="30"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -7196,7 +7195,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -7225,7 +7224,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -7253,7 +7252,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -7283,7 +7282,7 @@
       </c>
       <c r="I17" s="21"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -7312,7 +7311,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -7340,7 +7339,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21"/>
       <c r="B21" s="81"/>
       <c r="C21" s="21"/>
@@ -7351,7 +7350,7 @@
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="33" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21"/>
       <c r="B33" s="81"/>
       <c r="C33" s="21"/>
@@ -7362,7 +7361,7 @@
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
     </row>
-    <row r="37" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21"/>
       <c r="B37" s="81"/>
       <c r="C37" s="21"/>
@@ -7380,7 +7379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7390,19 +7389,19 @@
       <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="22.1640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7428,7 +7427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -7445,12 +7444,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -7475,7 +7474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -7501,7 +7500,7 @@
       </c>
       <c r="H5" s="42"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -7529,7 +7528,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -7557,7 +7556,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -7582,7 +7581,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -7610,7 +7609,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -7638,7 +7637,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -7662,7 +7661,7 @@
       </c>
       <c r="H11" s="42"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -7690,7 +7689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="53" t="s">
         <v>156</v>
       </c>
@@ -7718,7 +7717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -7728,7 +7727,7 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="31" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -7738,7 +7737,7 @@
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
     </row>
-    <row r="35" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -7748,7 +7747,7 @@
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
     </row>
-    <row r="39" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -7758,7 +7757,7 @@
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
     </row>
-    <row r="47" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -7768,8 +7767,8 @@
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="21"/>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -7779,7 +7778,7 @@
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
     </row>
-    <row r="63" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="21"/>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
@@ -7796,35 +7795,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" style="21" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="21"/>
+    <col min="2" max="4" width="11.5" style="21"/>
     <col min="5" max="6" width="0" style="129" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="21"/>
-    <col min="8" max="8" width="11.42578125" style="27"/>
-    <col min="9" max="9" width="9.85546875" style="21" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="21"/>
-    <col min="14" max="14" width="20.7109375" style="21" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="21" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="21"/>
-    <col min="17" max="17" width="12.42578125" style="81" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="21"/>
+    <col min="8" max="8" width="11.5" style="27"/>
+    <col min="9" max="9" width="9.83203125" style="21" customWidth="1"/>
+    <col min="10" max="13" width="11.5" style="21"/>
+    <col min="14" max="14" width="20.6640625" style="21" customWidth="1"/>
+    <col min="15" max="15" width="12.5" style="21" customWidth="1"/>
+    <col min="16" max="16" width="11.5" style="21"/>
+    <col min="17" max="17" width="12.5" style="81" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="0" style="81" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="55"/>
-    <col min="20" max="16384" width="11.42578125" style="21"/>
+    <col min="19" max="19" width="11.5" style="55"/>
+    <col min="20" max="16384" width="11.5" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7886,7 +7885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -7925,7 +7924,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -7935,7 +7934,7 @@
       <c r="E3" s="125"/>
       <c r="F3" s="125"/>
     </row>
-    <row r="4" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -7986,7 +7985,7 @@
       <c r="R4" s="37"/>
       <c r="S4" s="84"/>
     </row>
-    <row r="5" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -8046,7 +8045,7 @@
         <v>13.926959999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -8111,7 +8110,7 @@
         <v>13.926959999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -8176,7 +8175,7 @@
         <v>13.926959999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="53" t="s">
         <v>119</v>
       </c>
@@ -8235,7 +8234,7 @@
       </c>
       <c r="T8" s="26"/>
     </row>
-    <row r="9" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -8299,7 +8298,7 @@
         <v>11.0562</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -8368,7 +8367,7 @@
         <v>11.0562</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -8433,7 +8432,7 @@
       </c>
       <c r="T11" s="42"/>
     </row>
-    <row r="12" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -8501,7 +8500,7 @@
         <v>15.738</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="53" t="s">
         <v>156</v>
       </c>
@@ -8570,11 +8569,11 @@
       </c>
       <c r="T13" s="21"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H14" s="21"/>
       <c r="S14" s="118"/>
     </row>
-    <row r="17" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -8596,7 +8595,7 @@
       <c r="S17" s="55"/>
       <c r="T17" s="21"/>
     </row>
-    <row r="21" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -8618,7 +8617,7 @@
       <c r="S21" s="55"/>
       <c r="T21" s="21"/>
     </row>
-    <row r="25" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -8640,14 +8639,14 @@
       <c r="S25" s="55"/>
       <c r="T25" s="21"/>
     </row>
-    <row r="29" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E29" s="124"/>
       <c r="F29" s="124"/>
       <c r="Q29" s="116"/>
       <c r="R29" s="116"/>
       <c r="S29" s="64"/>
     </row>
-    <row r="33" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -8669,7 +8668,7 @@
       <c r="S33" s="55"/>
       <c r="T33" s="21"/>
     </row>
-    <row r="34" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -8691,7 +8690,7 @@
       <c r="S34" s="55"/>
       <c r="T34" s="21"/>
     </row>
-    <row r="41" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -8721,7 +8720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8731,24 +8730,24 @@
       <selection pane="bottomRight" activeCell="F1" sqref="F1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="81" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="81" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="81" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="81" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="21"/>
+    <col min="13" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -8789,7 +8788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -8809,7 +8808,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -8818,7 +8817,7 @@
       </c>
       <c r="C3" s="85"/>
     </row>
-    <row r="4" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -8855,7 +8854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -8901,7 +8900,7 @@
       </c>
       <c r="M5" s="42"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -8950,7 +8949,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -8999,7 +8998,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="62" t="s">
         <v>119</v>
       </c>
@@ -9045,7 +9044,7 @@
       </c>
       <c r="M8" s="42"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -9094,7 +9093,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -9143,7 +9142,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -9189,7 +9188,7 @@
       </c>
       <c r="M11" s="21"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -9238,7 +9237,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -9287,7 +9286,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="81"/>
@@ -9302,7 +9301,7 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
     </row>
-    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
       <c r="C18" s="81"/>
@@ -9317,7 +9316,7 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="22" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="81"/>
@@ -9332,7 +9331,7 @@
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
     </row>
-    <row r="26" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="81"/>
@@ -9347,7 +9346,7 @@
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
     </row>
-    <row r="30" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="81"/>
@@ -9362,7 +9361,7 @@
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
     </row>
-    <row r="34" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="81"/>
@@ -9377,7 +9376,7 @@
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
     </row>
-    <row r="38" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="81"/>
@@ -9399,27 +9398,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="36"/>
-    <col min="9" max="9" width="9.140625" style="36"/>
-    <col min="12" max="15" width="8.85546875" style="36"/>
+    <col min="1" max="1" width="21.5" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="8" width="8.83203125" style="36"/>
+    <col min="9" max="9" width="9.1640625" style="36"/>
+    <col min="12" max="15" width="8.83203125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -9469,7 +9468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9510,12 +9509,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>191</v>
       </c>
@@ -9554,7 +9553,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>199</v>
       </c>
@@ -9592,7 +9591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>197</v>
       </c>
@@ -9636,7 +9635,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>198</v>
       </c>
@@ -9679,7 +9678,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="139" t="s">
         <v>206</v>
       </c>
@@ -9712,7 +9711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="139" t="s">
         <v>207</v>
       </c>
@@ -9745,7 +9744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>3</v>
       </c>
@@ -9805,7 +9804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
         <v>150</v>
       </c>
@@ -9851,7 +9850,7 @@
       <c r="N11"/>
       <c r="O11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>151</v>
       </c>
@@ -9897,7 +9896,7 @@
       <c r="N12"/>
       <c r="O12"/>
     </row>
-    <row r="13" spans="1:16" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>154</v>
       </c>
@@ -9938,7 +9937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="62" t="s">
         <v>119</v>
       </c>
@@ -9984,7 +9983,7 @@
       <c r="N14"/>
       <c r="O14"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="53" t="s">
         <v>152</v>
       </c>
@@ -10030,7 +10029,7 @@
       <c r="N15"/>
       <c r="O15"/>
     </row>
-    <row r="16" spans="1:16" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
         <v>155</v>
       </c>
@@ -10071,7 +10070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="53" t="s">
         <v>120</v>
       </c>
@@ -10117,7 +10116,7 @@
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="53" t="s">
         <v>153</v>
       </c>
@@ -10163,7 +10162,7 @@
       <c r="N18"/>
       <c r="O18"/>
     </row>
-    <row r="19" spans="1:15" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" s="37" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="88" t="s">
         <v>156</v>
       </c>
@@ -10217,24 +10216,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10260,7 +10259,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -10283,19 +10282,19 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="29"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -10323,7 +10322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -10354,7 +10353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>143</v>
       </c>
@@ -10385,7 +10384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>144</v>
       </c>
@@ -10413,7 +10412,7 @@
         <v>0.22842009458374227</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>145</v>
       </c>
@@ -10445,7 +10444,7 @@
         <v>0.22842009458374227</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>146</v>
       </c>
@@ -10484,28 +10483,28 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="21" customWidth="1"/>
     <col min="9" max="9" width="19" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="21"/>
+    <col min="10" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10543,7 +10542,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -10569,7 +10568,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -10577,7 +10576,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -10612,7 +10611,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>147</v>
       </c>
@@ -10649,7 +10648,7 @@
         <v>4.2828767734451677E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>148</v>
       </c>
@@ -10687,7 +10686,7 @@
         <v>7.1381279557419458E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>149</v>
       </c>
@@ -10725,7 +10724,7 @@
         <v>7.1381279557419458E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>141</v>
       </c>
@@ -10766,7 +10765,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>142</v>
       </c>
@@ -10808,7 +10807,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>143</v>
       </c>
@@ -10850,7 +10849,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>144</v>
       </c>
@@ -10889,7 +10888,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>145</v>
       </c>
@@ -10931,7 +10930,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
wood chips for steam generation
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_var.xlsx
+++ b/data/steel/steel_simplified_var.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\steel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E45BD73-511C-EC49-8317-DB8201295DE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="598" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" tabRatio="598" firstSheet="4" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="17" r:id="rId1"/>
@@ -33,7 +32,7 @@
     <sheet name="CO2 Storage" sheetId="13" r:id="rId18"/>
     <sheet name="Ref" sheetId="7" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,12 +48,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
+    <comment ref="M5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,12 +117,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -152,12 +151,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -264,12 +263,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
+    <comment ref="K8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,12 +306,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000001000000}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1000,7 +999,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1487,8 +1486,8 @@
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1766,7 +1765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1776,18 +1775,18 @@
       <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="20.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -1810,7 +1809,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -1824,7 +1823,7 @@
       <c r="E2" s="55"/>
       <c r="F2" s="55"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -1836,7 +1835,7 @@
       <c r="E3" s="55"/>
       <c r="F3" s="55"/>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
@@ -1856,7 +1855,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -1878,7 +1877,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>151</v>
       </c>
@@ -1901,7 +1900,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="69" t="s">
         <v>154</v>
       </c>
@@ -1924,7 +1923,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -1946,7 +1945,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="69" t="s">
         <v>155</v>
       </c>
@@ -1992,7 +1991,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -2012,7 +2011,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -2058,7 +2057,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -2067,7 +2066,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
     </row>
-    <row r="30" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -2083,26 +2082,26 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2146,7 +2145,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2181,12 +2180,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -2231,7 +2230,7 @@
         <v>0.73399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -2279,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -2325,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>176</v>
       </c>
@@ -2380,7 +2379,7 @@
         <v>0.73399999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>141</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -2483,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>143</v>
       </c>
@@ -2539,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>144</v>
       </c>
@@ -2586,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>146</v>
       </c>
@@ -2706,22 +2705,22 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="21" customWidth="1"/>
     <col min="2" max="2" width="15" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -2741,7 +2740,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -2752,12 +2751,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -2765,7 +2764,7 @@
       <c r="C4" s="45"/>
       <c r="D4" s="45"/>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -2788,7 +2787,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -2838,7 +2837,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -2861,7 +2860,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -2886,7 +2885,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -2911,7 +2910,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -2959,7 +2958,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -2984,7 +2983,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -3007,7 +3006,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -3032,7 +3031,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -3057,7 +3056,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -3105,7 +3104,7 @@
         <v>no alloy</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -3136,26 +3135,26 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="21" customWidth="1"/>
     <col min="2" max="2" width="15" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.1640625" style="20"/>
+    <col min="6" max="6" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3169,7 +3168,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -3177,12 +3176,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -3194,7 +3193,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="45" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="38" t="s">
         <v>176</v>
       </c>
@@ -3233,7 +3232,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>150</v>
       </c>
@@ -3246,7 +3245,7 @@
       </c>
       <c r="D8" s="98"/>
     </row>
-    <row r="9" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>151</v>
       </c>
@@ -3259,7 +3258,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>154</v>
       </c>
@@ -3272,7 +3271,7 @@
         <v>1.3869182594347289</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>119</v>
       </c>
@@ -3285,7 +3284,7 @@
       </c>
       <c r="D11" s="98"/>
     </row>
-    <row r="12" spans="1:4" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>152</v>
       </c>
@@ -3299,7 +3298,7 @@
       </c>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:4" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>155</v>
       </c>
@@ -3313,7 +3312,7 @@
       </c>
       <c r="D13" s="45"/>
     </row>
-    <row r="14" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>120</v>
       </c>
@@ -3326,7 +3325,7 @@
       </c>
       <c r="D14" s="20"/>
     </row>
-    <row r="15" spans="1:4" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>153</v>
       </c>
@@ -3340,7 +3339,7 @@
       </c>
       <c r="D15" s="20"/>
     </row>
-    <row r="16" spans="1:4" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="63" t="s">
         <v>156</v>
       </c>
@@ -3354,7 +3353,7 @@
       </c>
       <c r="D16" s="45"/>
     </row>
-    <row r="17" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>141</v>
       </c>
@@ -3367,7 +3366,7 @@
       </c>
       <c r="D17" s="20"/>
     </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>142</v>
       </c>
@@ -3381,7 +3380,7 @@
       </c>
       <c r="D18" s="20"/>
     </row>
-    <row r="19" spans="1:4" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>143</v>
       </c>
@@ -3395,7 +3394,7 @@
       </c>
       <c r="D19" s="45"/>
     </row>
-    <row r="20" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>144</v>
       </c>
@@ -3408,7 +3407,7 @@
       </c>
       <c r="D20" s="20"/>
     </row>
-    <row r="21" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>145</v>
       </c>
@@ -3422,7 +3421,7 @@
       </c>
       <c r="D21" s="20"/>
     </row>
-    <row r="22" spans="1:4" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
         <v>146</v>
       </c>
@@ -3436,58 +3435,58 @@
       </c>
       <c r="D22" s="45"/>
     </row>
-    <row r="23" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
     </row>
-    <row r="25" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
     </row>
-    <row r="26" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
     </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
     </row>
-    <row r="28" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
     </row>
-    <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
     </row>
-    <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
     </row>
-    <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
     </row>
-    <row r="32" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
     </row>
-    <row r="36" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -3500,28 +3499,28 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="20" customWidth="1"/>
     <col min="5" max="5" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.1640625" style="20"/>
+    <col min="10" max="16384" width="10.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3545,7 +3544,7 @@
       <c r="I1" s="42"/>
       <c r="J1" s="42"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -3557,12 +3556,12 @@
       </c>
       <c r="G2" s="99"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -3578,7 +3577,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -3594,7 +3593,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -3610,7 +3609,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="45" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>176</v>
       </c>
@@ -3626,7 +3625,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>150</v>
       </c>
@@ -3640,7 +3639,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>151</v>
       </c>
@@ -3656,7 +3655,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>154</v>
       </c>
@@ -3672,7 +3671,7 @@
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>119</v>
       </c>
@@ -3692,7 +3691,7 @@
       <c r="I11" s="82"/>
       <c r="J11" s="82"/>
     </row>
-    <row r="12" spans="1:10" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>152</v>
       </c>
@@ -3715,7 +3714,7 @@
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
     </row>
-    <row r="13" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>155</v>
       </c>
@@ -3738,7 +3737,7 @@
       <c r="I13" s="45"/>
       <c r="J13" s="45"/>
     </row>
-    <row r="14" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>120</v>
       </c>
@@ -3758,7 +3757,7 @@
       <c r="I14" s="82"/>
       <c r="J14" s="82"/>
     </row>
-    <row r="15" spans="1:10" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>153</v>
       </c>
@@ -3781,7 +3780,7 @@
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="1:10" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="63" t="s">
         <v>156</v>
       </c>
@@ -3804,7 +3803,7 @@
       <c r="I16" s="45"/>
       <c r="J16" s="45"/>
     </row>
-    <row r="17" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>141</v>
       </c>
@@ -3824,7 +3823,7 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>142</v>
       </c>
@@ -3847,7 +3846,7 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>143</v>
       </c>
@@ -3870,7 +3869,7 @@
       <c r="I19" s="45"/>
       <c r="J19" s="45"/>
     </row>
-    <row r="20" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>144</v>
       </c>
@@ -3890,7 +3889,7 @@
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>145</v>
       </c>
@@ -3913,7 +3912,7 @@
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="22" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
         <v>146</v>
       </c>
@@ -3936,7 +3935,7 @@
       <c r="I22" s="45"/>
       <c r="J22" s="45"/>
     </row>
-    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
@@ -3947,7 +3946,7 @@
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -3959,7 +3958,7 @@
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
@@ -3970,7 +3969,7 @@
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
@@ -3981,7 +3980,7 @@
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
@@ -3992,7 +3991,7 @@
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -4004,7 +4003,7 @@
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
@@ -4015,7 +4014,7 @@
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
@@ -4026,7 +4025,7 @@
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
     </row>
-    <row r="31" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
@@ -4037,7 +4036,7 @@
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
     </row>
-    <row r="32" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -4049,8 +4048,8 @@
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -4062,7 +4061,7 @@
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
     </row>
-    <row r="40" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -4074,8 +4073,8 @@
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
     </row>
-    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
@@ -4094,27 +4093,27 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="20" customWidth="1"/>
-    <col min="5" max="7" width="15.83203125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="54" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="20" customWidth="1"/>
+    <col min="5" max="7" width="15.85546875" style="20" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="54" customWidth="1"/>
     <col min="9" max="9" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="21"/>
+    <col min="10" max="10" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -4143,7 +4142,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -4157,12 +4156,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -4176,7 +4175,7 @@
       <c r="I4" s="45"/>
       <c r="J4" s="45"/>
     </row>
-    <row r="5" spans="1:10" s="42" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="42" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -4192,15 +4191,15 @@
       <c r="E5" s="42">
         <v>0</v>
       </c>
-      <c r="F5" s="27" t="s">
-        <v>113</v>
+      <c r="F5" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="H5" s="90">
         <f>(25.3/4.6668)*Ref!B$18</f>
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -4219,8 +4218,8 @@
       <c r="E6" s="51">
         <v>1</v>
       </c>
-      <c r="F6" s="27" t="s">
-        <v>113</v>
+      <c r="F6" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="90">
@@ -4230,7 +4229,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
     </row>
-    <row r="7" spans="1:10" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -4249,15 +4248,15 @@
       <c r="E7" s="51">
         <v>1</v>
       </c>
-      <c r="F7" s="27" t="s">
-        <v>113</v>
+      <c r="F7" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="H7" s="78">
         <f>H5</f>
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -4273,8 +4272,8 @@
       <c r="E8" s="42">
         <v>0</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>113</v>
+      <c r="F8" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G8" s="42"/>
       <c r="H8" s="90">
@@ -4282,7 +4281,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -4301,8 +4300,8 @@
       <c r="E9" s="51">
         <v>1</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>113</v>
+      <c r="F9" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="90">
@@ -4312,7 +4311,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -4331,8 +4330,8 @@
       <c r="E10" s="51">
         <v>1</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>113</v>
+      <c r="F10" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G10" s="38"/>
       <c r="H10" s="78">
@@ -4342,7 +4341,7 @@
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -4358,8 +4357,8 @@
       <c r="E11" s="42">
         <v>0</v>
       </c>
-      <c r="F11" s="27" t="s">
-        <v>113</v>
+      <c r="F11" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G11" s="42"/>
       <c r="H11" s="90">
@@ -4367,7 +4366,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -4385,8 +4384,8 @@
       <c r="E12" s="51">
         <v>1</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>113</v>
+      <c r="F12" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="90">
@@ -4394,7 +4393,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -4412,8 +4411,8 @@
       <c r="E13" s="51">
         <v>1</v>
       </c>
-      <c r="F13" s="27" t="s">
-        <v>113</v>
+      <c r="F13" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G13" s="38"/>
       <c r="H13" s="78">
@@ -4423,7 +4422,7 @@
       <c r="I13" s="45"/>
       <c r="J13" s="45"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -4439,8 +4438,8 @@
       <c r="E14" s="42">
         <v>0</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>169</v>
+      <c r="F14" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G14" s="42"/>
       <c r="H14" s="90">
@@ -4450,7 +4449,7 @@
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -4469,8 +4468,8 @@
       <c r="E15" s="51">
         <v>1</v>
       </c>
-      <c r="F15" s="27" t="s">
-        <v>169</v>
+      <c r="F15" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="90">
@@ -4478,7 +4477,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -4496,8 +4495,8 @@
       <c r="E16" s="51">
         <v>1</v>
       </c>
-      <c r="F16" s="27" t="s">
-        <v>169</v>
+      <c r="F16" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="78">
@@ -4507,7 +4506,7 @@
       <c r="I16" s="45"/>
       <c r="J16" s="45"/>
     </row>
-    <row r="17" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -4523,8 +4522,8 @@
       <c r="E17" s="42">
         <v>0</v>
       </c>
-      <c r="F17" s="27" t="s">
-        <v>169</v>
+      <c r="F17" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="H17" s="90">
         <f>(25.3/4.6668)*Ref!B$18</f>
@@ -4533,7 +4532,7 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -4552,8 +4551,8 @@
       <c r="E18" s="51">
         <v>1</v>
       </c>
-      <c r="F18" s="27" t="s">
-        <v>169</v>
+      <c r="F18" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="90">
@@ -4561,7 +4560,7 @@
         <v>1.9516585240421703E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -4579,8 +4578,8 @@
       <c r="E19" s="51">
         <v>1</v>
       </c>
-      <c r="F19" s="27" t="s">
-        <v>169</v>
+      <c r="F19" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="G19" s="38"/>
       <c r="H19" s="78">
@@ -4590,7 +4589,7 @@
       <c r="I19" s="45"/>
       <c r="J19" s="45"/>
     </row>
-    <row r="21" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -4602,7 +4601,7 @@
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="25" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -4614,7 +4613,7 @@
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4622,7 +4621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4632,16 +4631,16 @@
       <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="21" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" style="21"/>
-    <col min="6" max="6" width="8.83203125" style="96"/>
-    <col min="7" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="26.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="21" customWidth="1"/>
+    <col min="3" max="5" width="8.85546875" style="21"/>
+    <col min="6" max="6" width="8.85546875" style="96"/>
+    <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -4664,7 +4663,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -4685,7 +4684,7 @@
       </c>
       <c r="G2" s="106"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
@@ -4700,7 +4699,7 @@
       <c r="F3" s="115"/>
       <c r="G3" s="106"/>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -4721,7 +4720,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -4745,7 +4744,7 @@
       </c>
       <c r="G5" s="105"/>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -4770,7 +4769,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -4795,7 +4794,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>119</v>
       </c>
@@ -4817,7 +4816,7 @@
       </c>
       <c r="G8" s="108"/>
     </row>
-    <row r="9" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -4843,7 +4842,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -4868,7 +4867,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -4892,7 +4891,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -4917,7 +4916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -4943,7 +4942,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -4969,7 +4968,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -4994,7 +4993,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -5019,7 +5018,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -5071,7 +5070,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -5099,7 +5098,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -5108,7 +5107,7 @@
       <c r="F21" s="96"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5117,7 +5116,7 @@
       <c r="F25" s="96"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -5126,7 +5125,7 @@
       <c r="F33" s="96"/>
       <c r="G33" s="21"/>
     </row>
-    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -5142,7 +5141,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5152,16 +5151,16 @@
       <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="21" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" style="21"/>
-    <col min="6" max="6" width="8.83203125" style="96"/>
-    <col min="7" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="26.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="21" customWidth="1"/>
+    <col min="3" max="5" width="8.85546875" style="21"/>
+    <col min="6" max="6" width="8.85546875" style="96"/>
+    <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -5184,7 +5183,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -5205,7 +5204,7 @@
       </c>
       <c r="G2" s="106"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
@@ -5220,7 +5219,7 @@
       <c r="F3" s="115"/>
       <c r="G3" s="106"/>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -5239,7 +5238,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="111"/>
     </row>
-    <row r="5" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -5263,7 +5262,7 @@
       </c>
       <c r="G5" s="105"/>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -5288,7 +5287,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -5313,7 +5312,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>119</v>
       </c>
@@ -5337,7 +5336,7 @@
       </c>
       <c r="G8" s="108"/>
     </row>
-    <row r="9" spans="1:7" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -5363,7 +5362,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -5388,7 +5387,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -5411,7 +5410,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -5436,7 +5435,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -5462,7 +5461,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -5486,7 +5485,7 @@
       </c>
       <c r="G14" s="105"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -5511,7 +5510,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -5536,7 +5535,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -5560,7 +5559,7 @@
       </c>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -5585,7 +5584,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -5611,7 +5610,7 @@
       </c>
       <c r="G19" s="21"/>
     </row>
-    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -5620,7 +5619,7 @@
       <c r="F21" s="96"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5629,7 +5628,7 @@
       <c r="F25" s="96"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -5638,7 +5637,7 @@
       <c r="F33" s="96"/>
       <c r="G33" s="21"/>
     </row>
-    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -5654,16 +5653,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -5674,7 +5673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -5685,7 +5684,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
@@ -5694,7 +5693,7 @@
       </c>
       <c r="C3" s="106"/>
     </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -5705,7 +5704,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -5717,7 +5716,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -5730,7 +5729,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -5743,7 +5742,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>119</v>
       </c>
@@ -5755,7 +5754,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -5768,7 +5767,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -5781,7 +5780,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -5793,7 +5792,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -5806,7 +5805,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -5819,7 +5818,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -5831,7 +5830,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -5844,7 +5843,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -5857,7 +5856,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -5869,7 +5868,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -5882,7 +5881,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -5901,20 +5900,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="21" customWidth="1"/>
-    <col min="2" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="19.140625" style="21" customWidth="1"/>
+    <col min="2" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>77</v>
       </c>
@@ -5931,7 +5930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>72</v>
       </c>
@@ -5945,12 +5944,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="109" t="s">
         <v>3</v>
       </c>
@@ -5968,7 +5967,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -5986,7 +5985,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -6007,7 +6006,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -6028,7 +6027,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -6047,7 +6046,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -6068,7 +6067,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="69" t="s">
         <v>155</v>
       </c>
@@ -6088,7 +6087,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -6107,7 +6106,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -6128,7 +6127,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -6149,7 +6148,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
@@ -6168,7 +6167,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>142</v>
       </c>
@@ -6189,7 +6188,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -6210,7 +6209,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
@@ -6228,7 +6227,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>145</v>
       </c>
@@ -6249,7 +6248,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="70" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -6270,22 +6269,22 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
     </row>
-    <row r="27" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
     </row>
-    <row r="31" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
     </row>
-    <row r="35" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -6296,33 +6295,33 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>29</v>
@@ -6331,7 +6330,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>31</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>5.3537967341839917E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
@@ -6355,7 +6354,7 @@
         <v>7.1573391630231102E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>33</v>
       </c>
@@ -6367,7 +6366,7 @@
         <v>1.2496698492013921E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>34</v>
       </c>
@@ -6379,7 +6378,7 @@
         <v>1.963482644775587E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>35</v>
       </c>
@@ -6391,7 +6390,7 @@
         <v>8.9938431337556905E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>36</v>
       </c>
@@ -6403,7 +6402,7 @@
         <v>8.0375122691175155E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
@@ -6416,7 +6415,7 @@
         <v>4.1190030040748338E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
@@ -6428,7 +6427,7 @@
         <v>1.2498170786115822E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>39</v>
       </c>
@@ -6440,24 +6439,24 @@
         <v>1.4276255911483892E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="16" t="s">
         <v>41</v>
@@ -6465,7 +6464,7 @@
       <c r="C16" s="16"/>
       <c r="H16" s="122"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>42</v>
       </c>
@@ -6474,7 +6473,7 @@
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>43</v>
       </c>
@@ -6486,7 +6485,7 @@
       <c r="D18" s="23"/>
       <c r="E18" s="122"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>44</v>
       </c>
@@ -6496,7 +6495,7 @@
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>71</v>
       </c>
@@ -6506,7 +6505,7 @@
       </c>
       <c r="E20" s="122"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>73</v>
       </c>
@@ -6515,7 +6514,7 @@
         <v>0.90718581887127947</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>214</v>
       </c>
@@ -6527,7 +6526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6537,17 +6536,17 @@
       <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.83203125" style="81" customWidth="1"/>
-    <col min="6" max="6" width="63.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="19.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="81" customWidth="1"/>
+    <col min="6" max="6" width="63.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -6567,7 +6566,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -6578,12 +6577,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
@@ -6596,7 +6595,7 @@
       <c r="D4" s="37"/>
       <c r="E4" s="37"/>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -6610,7 +6609,7 @@
       <c r="D5" s="59"/>
       <c r="E5" s="59"/>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -6623,7 +6622,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -6638,7 +6637,7 @@
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
     </row>
-    <row r="8" spans="1:6" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -6653,7 +6652,7 @@
       <c r="E8" s="81"/>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -6666,7 +6665,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="69" t="s">
         <v>155</v>
       </c>
@@ -6681,7 +6680,7 @@
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -6692,7 +6691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -6705,7 +6704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -6720,7 +6719,7 @@
       <c r="D13" s="37"/>
       <c r="E13" s="37"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -6732,7 +6731,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -6745,7 +6744,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -6760,7 +6759,7 @@
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -6772,7 +6771,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -6785,7 +6784,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -6801,7 +6800,7 @@
       <c r="E19" s="37"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A26:F49">
+  <sortState ref="A26:F49">
     <sortCondition ref="A26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6810,7 +6809,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6820,19 +6819,19 @@
       <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="81" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="21" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="20.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="81" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -6861,7 +6860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -6872,13 +6871,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="85"/>
     </row>
-    <row r="4" spans="1:9" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -6903,7 +6902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -6932,7 +6931,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -6962,7 +6961,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -6991,7 +6990,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -7020,7 +7019,7 @@
       </c>
       <c r="I8" s="42"/>
     </row>
-    <row r="9" spans="1:9" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -7051,7 +7050,7 @@
       </c>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:9" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -7080,7 +7079,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -7106,7 +7105,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -7136,7 +7135,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="70" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -7166,7 +7165,7 @@
       </c>
       <c r="I13" s="30"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -7195,7 +7194,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -7224,7 +7223,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>143</v>
       </c>
@@ -7252,7 +7251,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -7282,7 +7281,7 @@
       </c>
       <c r="I17" s="21"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -7311,7 +7310,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>146</v>
       </c>
@@ -7339,7 +7338,7 @@
         <v>0.25098039215686274</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="81"/>
       <c r="C21" s="21"/>
@@ -7350,7 +7349,7 @@
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="33" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="81"/>
       <c r="C33" s="21"/>
@@ -7361,7 +7360,7 @@
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
     </row>
-    <row r="37" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="81"/>
       <c r="C37" s="21"/>
@@ -7379,7 +7378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7389,19 +7388,19 @@
       <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="22.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7427,7 +7426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -7444,12 +7443,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -7474,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -7500,7 +7499,7 @@
       </c>
       <c r="H5" s="42"/>
     </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -7528,7 +7527,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -7556,7 +7555,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
@@ -7581,7 +7580,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
@@ -7609,7 +7608,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -7637,7 +7636,7 @@
         <v>0.1152</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -7661,7 +7660,7 @@
       </c>
       <c r="H11" s="42"/>
     </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -7689,7 +7688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
         <v>156</v>
       </c>
@@ -7717,7 +7716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -7727,7 +7726,7 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="31" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -7737,7 +7736,7 @@
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
     </row>
-    <row r="35" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -7747,7 +7746,7 @@
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
     </row>
-    <row r="39" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -7757,7 +7756,7 @@
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
     </row>
-    <row r="47" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -7767,8 +7766,8 @@
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -7778,7 +7777,7 @@
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
     </row>
-    <row r="63" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
@@ -7795,7 +7794,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7805,25 +7804,25 @@
       <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" style="21" customWidth="1"/>
-    <col min="2" max="4" width="11.5" style="21"/>
+    <col min="2" max="4" width="11.42578125" style="21"/>
     <col min="5" max="6" width="0" style="129" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="21"/>
-    <col min="8" max="8" width="11.5" style="27"/>
-    <col min="9" max="9" width="9.83203125" style="21" customWidth="1"/>
-    <col min="10" max="13" width="11.5" style="21"/>
-    <col min="14" max="14" width="20.6640625" style="21" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="21" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="21"/>
-    <col min="17" max="17" width="12.5" style="81" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="21"/>
+    <col min="8" max="8" width="11.42578125" style="27"/>
+    <col min="9" max="9" width="9.85546875" style="21" customWidth="1"/>
+    <col min="10" max="13" width="11.42578125" style="21"/>
+    <col min="14" max="14" width="20.7109375" style="21" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="21" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="21"/>
+    <col min="17" max="17" width="12.42578125" style="81" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="0" style="81" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5" style="55"/>
-    <col min="20" max="16384" width="11.5" style="21"/>
+    <col min="19" max="19" width="11.42578125" style="55"/>
+    <col min="20" max="16384" width="11.42578125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7885,7 +7884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -7924,7 +7923,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -7934,7 +7933,7 @@
       <c r="E3" s="125"/>
       <c r="F3" s="125"/>
     </row>
-    <row r="4" spans="1:20" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -7985,7 +7984,7 @@
       <c r="R4" s="37"/>
       <c r="S4" s="84"/>
     </row>
-    <row r="5" spans="1:20" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -8045,7 +8044,7 @@
         <v>13.926959999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -8110,7 +8109,7 @@
         <v>13.926959999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -8175,7 +8174,7 @@
         <v>13.926959999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
         <v>119</v>
       </c>
@@ -8234,7 +8233,7 @@
       </c>
       <c r="T8" s="26"/>
     </row>
-    <row r="9" spans="1:20" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -8298,7 +8297,7 @@
         <v>11.0562</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -8367,7 +8366,7 @@
         <v>11.0562</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
@@ -8432,7 +8431,7 @@
       </c>
       <c r="T11" s="42"/>
     </row>
-    <row r="12" spans="1:20" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -8500,7 +8499,7 @@
         <v>15.738</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
         <v>156</v>
       </c>
@@ -8569,11 +8568,11 @@
       </c>
       <c r="T13" s="21"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H14" s="21"/>
       <c r="S14" s="118"/>
     </row>
-    <row r="17" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -8595,7 +8594,7 @@
       <c r="S17" s="55"/>
       <c r="T17" s="21"/>
     </row>
-    <row r="21" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -8617,7 +8616,7 @@
       <c r="S21" s="55"/>
       <c r="T21" s="21"/>
     </row>
-    <row r="25" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -8639,14 +8638,14 @@
       <c r="S25" s="55"/>
       <c r="T25" s="21"/>
     </row>
-    <row r="29" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E29" s="124"/>
       <c r="F29" s="124"/>
       <c r="Q29" s="116"/>
       <c r="R29" s="116"/>
       <c r="S29" s="64"/>
     </row>
-    <row r="33" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -8668,7 +8667,7 @@
       <c r="S33" s="55"/>
       <c r="T33" s="21"/>
     </row>
-    <row r="34" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -8690,7 +8689,7 @@
       <c r="S34" s="55"/>
       <c r="T34" s="21"/>
     </row>
-    <row r="41" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -8720,7 +8719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8730,24 +8729,24 @@
       <selection pane="bottomRight" activeCell="F1" sqref="F1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="81" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="81" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="81" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="81" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="21"/>
+    <col min="13" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -8788,7 +8787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -8808,7 +8807,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -8817,7 +8816,7 @@
       </c>
       <c r="C3" s="85"/>
     </row>
-    <row r="4" spans="1:13" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -8854,7 +8853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
@@ -8900,7 +8899,7 @@
       </c>
       <c r="M5" s="42"/>
     </row>
-    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
@@ -8949,7 +8948,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
@@ -8998,7 +8997,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>119</v>
       </c>
@@ -9044,7 +9043,7 @@
       </c>
       <c r="M8" s="42"/>
     </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>152</v>
       </c>
@@ -9093,7 +9092,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
@@ -9142,7 +9141,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
@@ -9188,7 +9187,7 @@
       </c>
       <c r="M11" s="21"/>
     </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
@@ -9237,7 +9236,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
@@ -9286,7 +9285,7 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="81"/>
@@ -9301,7 +9300,7 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
     </row>
-    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
       <c r="C18" s="81"/>
@@ -9316,7 +9315,7 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="22" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="81"/>
@@ -9331,7 +9330,7 @@
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
     </row>
-    <row r="26" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="81"/>
@@ -9346,7 +9345,7 @@
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
     </row>
-    <row r="30" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="81"/>
@@ -9361,7 +9360,7 @@
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
     </row>
-    <row r="34" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="81"/>
@@ -9376,7 +9375,7 @@
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
     </row>
-    <row r="38" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="81"/>
@@ -9398,27 +9397,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="8" width="8.83203125" style="36"/>
-    <col min="9" max="9" width="9.1640625" style="36"/>
-    <col min="12" max="15" width="8.83203125" style="36"/>
+    <col min="1" max="1" width="21.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="36"/>
+    <col min="9" max="9" width="9.140625" style="36"/>
+    <col min="12" max="15" width="8.85546875" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -9468,7 +9467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9509,12 +9508,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>191</v>
       </c>
@@ -9553,7 +9552,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>199</v>
       </c>
@@ -9591,7 +9590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>197</v>
       </c>
@@ -9635,7 +9634,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>198</v>
       </c>
@@ -9678,7 +9677,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="139" t="s">
         <v>206</v>
       </c>
@@ -9711,7 +9710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="139" t="s">
         <v>207</v>
       </c>
@@ -9744,7 +9743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>3</v>
       </c>
@@ -9804,7 +9803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>150</v>
       </c>
@@ -9850,7 +9849,7 @@
       <c r="N11"/>
       <c r="O11"/>
     </row>
-    <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>151</v>
       </c>
@@ -9896,7 +9895,7 @@
       <c r="N12"/>
       <c r="O12"/>
     </row>
-    <row r="13" spans="1:16" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>154</v>
       </c>
@@ -9937,7 +9936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>119</v>
       </c>
@@ -9983,7 +9982,7 @@
       <c r="N14"/>
       <c r="O14"/>
     </row>
-    <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>152</v>
       </c>
@@ -10029,7 +10028,7 @@
       <c r="N15"/>
       <c r="O15"/>
     </row>
-    <row r="16" spans="1:16" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="63" t="s">
         <v>155</v>
       </c>
@@ -10070,7 +10069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
         <v>120</v>
       </c>
@@ -10116,7 +10115,7 @@
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
         <v>153</v>
       </c>
@@ -10162,7 +10161,7 @@
       <c r="N18"/>
       <c r="O18"/>
     </row>
-    <row r="19" spans="1:15" s="37" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="88" t="s">
         <v>156</v>
       </c>
@@ -10216,24 +10215,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10259,7 +10258,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -10282,19 +10281,19 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="29"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -10322,7 +10321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -10353,7 +10352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>143</v>
       </c>
@@ -10384,7 +10383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>144</v>
       </c>
@@ -10412,7 +10411,7 @@
         <v>0.22842009458374227</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>145</v>
       </c>
@@ -10444,7 +10443,7 @@
         <v>0.22842009458374227</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>146</v>
       </c>
@@ -10483,28 +10482,28 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="21" customWidth="1"/>
     <col min="9" max="9" width="19" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="21"/>
+    <col min="10" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10542,7 +10541,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
@@ -10568,7 +10567,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
@@ -10576,7 +10575,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -10611,7 +10610,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>147</v>
       </c>
@@ -10648,7 +10647,7 @@
         <v>4.2828767734451677E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>148</v>
       </c>
@@ -10686,7 +10685,7 @@
         <v>7.1381279557419458E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>149</v>
       </c>
@@ -10724,7 +10723,7 @@
         <v>7.1381279557419458E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>141</v>
       </c>
@@ -10765,7 +10764,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>142</v>
       </c>
@@ -10807,7 +10806,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>143</v>
       </c>
@@ -10849,7 +10848,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>144</v>
       </c>
@@ -10888,7 +10887,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>145</v>
       </c>
@@ -10930,7 +10929,7 @@
         <v>1.5165898340948458E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="30" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
change electricity use for HIsarna
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_var.xlsx
+++ b/data/steel/steel_simplified_var.xlsx
@@ -1397,7 +1397,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1479,6 +1478,7 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2264,7 +2264,7 @@
         <f>0.027/1.15*Ref!B18*1000</f>
         <v>8.4521739130434786E-2</v>
       </c>
-      <c r="L5" s="121">
+      <c r="L5" s="120">
         <f>J5*0.0016</f>
         <v>0</v>
       </c>
@@ -2310,7 +2310,7 @@
       <c r="K6" s="41">
         <v>0</v>
       </c>
-      <c r="L6" s="121">
+      <c r="L6" s="120">
         <f>J6*0.0015</f>
         <v>1.8600000000000001E-3</v>
       </c>
@@ -2363,7 +2363,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L7" s="123">
+      <c r="L7" s="122">
         <f>J7*0.0015</f>
         <v>7.0500000000000001E-4</v>
       </c>
@@ -2412,11 +2412,11 @@
         <f>J8*90*Ref!B$18</f>
         <v>0.40175999999999995</v>
       </c>
-      <c r="L8" s="131">
+      <c r="L8" s="130">
         <f>J8*0.0015</f>
         <v>1.8600000000000001E-3</v>
       </c>
-      <c r="M8" s="132">
+      <c r="M8" s="131">
         <v>2</v>
       </c>
       <c r="N8" s="42">
@@ -2435,7 +2435,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D9" s="119">
+      <c r="D9" s="118">
         <v>0.5</v>
       </c>
       <c r="E9" t="str">
@@ -2466,7 +2466,7 @@
         <f t="shared" si="1"/>
         <v>0.40175999999999995</v>
       </c>
-      <c r="L9" s="122">
+      <c r="L9" s="121">
         <f t="shared" si="1"/>
         <v>1.8600000000000001E-3</v>
       </c>
@@ -2522,7 +2522,7 @@
         <f t="shared" si="2"/>
         <v>0.40175999999999995</v>
       </c>
-      <c r="L10" s="123">
+      <c r="L10" s="122">
         <f t="shared" si="2"/>
         <v>1.8600000000000001E-3</v>
       </c>
@@ -2571,11 +2571,11 @@
         <f>J11*90*Ref!B$18</f>
         <v>0.40175999999999995</v>
       </c>
-      <c r="L11" s="131">
+      <c r="L11" s="130">
         <f>J11*0.0015</f>
         <v>1.8600000000000001E-3</v>
       </c>
-      <c r="M11" s="132">
+      <c r="M11" s="131">
         <v>2</v>
       </c>
       <c r="N11" s="42">
@@ -2594,7 +2594,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D12" s="119">
+      <c r="D12" s="118">
         <v>0.5</v>
       </c>
       <c r="E12" t="str">
@@ -2625,7 +2625,7 @@
         <f t="shared" si="3"/>
         <v>0.40175999999999995</v>
       </c>
-      <c r="L12" s="122">
+      <c r="L12" s="121">
         <f t="shared" si="3"/>
         <v>1.8600000000000001E-3</v>
       </c>
@@ -2681,7 +2681,7 @@
         <f t="shared" si="4"/>
         <v>0.40175999999999995</v>
       </c>
-      <c r="L13" s="123">
+      <c r="L13" s="122">
         <f t="shared" si="4"/>
         <v>1.8600000000000001E-3</v>
       </c>
@@ -2724,7 +2724,7 @@
       <c r="B1" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="95" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="42" t="s">
@@ -2765,7 +2765,7 @@
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="97">
+      <c r="B5" s="96">
         <f>(2.1+2.1+2.6)*Ref!$C$12</f>
         <v>9.7078540198090469E-3</v>
       </c>
@@ -2773,7 +2773,7 @@
         <f>(10.3+25+105.3)*Ref!B$18</f>
         <v>0.50615999999999994</v>
       </c>
-      <c r="D5" s="113">
+      <c r="D5" s="112">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E5">
@@ -2838,7 +2838,7 @@
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="97">
+      <c r="B8" s="96">
         <f>(2.1+2.1+2.6)*Ref!$C$12</f>
         <v>9.7078540198090469E-3</v>
       </c>
@@ -2846,7 +2846,7 @@
         <f>(10.3+25+105.3)*Ref!B$18</f>
         <v>0.50615999999999994</v>
       </c>
-      <c r="D8" s="113">
+      <c r="D8" s="112">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E8">
@@ -2911,7 +2911,7 @@
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="97">
+      <c r="B11" s="96">
         <f>(2.1+2.1+2.6)*Ref!$C$12</f>
         <v>9.7078540198090469E-3</v>
       </c>
@@ -2919,7 +2919,7 @@
         <f>(10.3+25+105.3)*Ref!B$18</f>
         <v>0.50615999999999994</v>
       </c>
-      <c r="D11" s="113">
+      <c r="D11" s="112">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E11">
@@ -2984,7 +2984,7 @@
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="97">
+      <c r="B14" s="96">
         <f>(2.1+2.1+2.6)*Ref!$C$12</f>
         <v>9.7078540198090469E-3</v>
       </c>
@@ -2992,7 +2992,7 @@
         <f>(10.3+25+105.3)*Ref!B$18</f>
         <v>0.50615999999999994</v>
       </c>
-      <c r="D14" s="113">
+      <c r="D14" s="112">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E14">
@@ -3057,7 +3057,7 @@
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="97">
+      <c r="B17" s="96">
         <f>(2.1+2.1+2.6)*Ref!$C$12</f>
         <v>9.7078540198090469E-3</v>
       </c>
@@ -3065,7 +3065,7 @@
         <f>(10.3+25+105.3)*Ref!B$18</f>
         <v>0.50615999999999994</v>
       </c>
-      <c r="D17" s="113">
+      <c r="D17" s="112">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E17">
@@ -3158,7 +3158,7 @@
       <c r="B1" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="95" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="42" t="s">
@@ -3182,7 +3182,7 @@
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="97">
+      <c r="B4" s="96">
         <v>0.9</v>
       </c>
       <c r="C4" s="57">
@@ -3194,7 +3194,7 @@
       <c r="A5" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="B5" s="97">
+      <c r="B5" s="96">
         <f>B4</f>
         <v>0.9</v>
       </c>
@@ -3207,7 +3207,7 @@
       <c r="A6" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="B6" s="97">
+      <c r="B6" s="96">
         <f>B4</f>
         <v>0.9</v>
       </c>
@@ -3224,7 +3224,7 @@
         <f>B4</f>
         <v>0.9</v>
       </c>
-      <c r="C7" s="120">
+      <c r="C7" s="119">
         <f>C4</f>
         <v>1.3869182594347289</v>
       </c>
@@ -3233,14 +3233,14 @@
       <c r="A8" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="97">
+      <c r="B8" s="96">
         <v>0.9</v>
       </c>
       <c r="C8" s="57">
         <f>0.55*Ref!B$18/Ref!$C$12</f>
         <v>1.3869182594347289</v>
       </c>
-      <c r="D8" s="98"/>
+      <c r="D8" s="97"/>
     </row>
     <row r="9" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
@@ -3272,14 +3272,14 @@
       <c r="A11" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="97">
+      <c r="B11" s="96">
         <v>0.9</v>
       </c>
-      <c r="C11" s="97">
+      <c r="C11" s="96">
         <f>(0.55*Ref!B18/Ref!C12*(38/158.3))+(0.47*Ref!B18/Ref!C12*(120.3/158.3))</f>
         <v>1.2336109450282529</v>
       </c>
-      <c r="D11" s="98"/>
+      <c r="D11" s="97"/>
     </row>
     <row r="12" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
@@ -3316,7 +3316,7 @@
       <c r="B14" s="20">
         <v>0.9</v>
       </c>
-      <c r="C14" s="97">
+      <c r="C14" s="96">
         <f>(0.55*Ref!B18/Ref!C12*(38/158.3))+(0.47*Ref!B18/Ref!C12*(120.3/158.3))</f>
         <v>1.2336109450282529</v>
       </c>
@@ -3521,10 +3521,10 @@
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="98" t="s">
         <v>75</v>
       </c>
       <c r="D1" s="42" t="s">
@@ -3551,7 +3551,7 @@
       <c r="C2" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="99"/>
+      <c r="G2" s="98"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
@@ -3598,7 +3598,7 @@
         <f>B4</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C6" s="130">
+      <c r="C6" s="129">
         <v>0</v>
       </c>
       <c r="D6" s="54" t="str">
@@ -3617,7 +3617,7 @@
       <c r="C7" s="46">
         <v>0</v>
       </c>
-      <c r="D7" s="112" t="str">
+      <c r="D7" s="111" t="str">
         <f>D4</f>
         <v>natural gas - IPCC</v>
       </c>
@@ -3626,13 +3626,13 @@
       <c r="A8" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="82">
+      <c r="B8" s="81">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C8" s="141">
-        <v>0</v>
-      </c>
-      <c r="D8" s="82" t="s">
+      <c r="C8" s="140">
+        <v>0</v>
+      </c>
+      <c r="D8" s="81" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3640,10 +3640,10 @@
       <c r="A9" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="82">
+      <c r="B9" s="81">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C9" s="142">
+      <c r="C9" s="141">
         <f t="shared" ref="C9" si="0">C$8</f>
         <v>0</v>
       </c>
@@ -3656,10 +3656,10 @@
       <c r="A10" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="83">
+      <c r="B10" s="82">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C10" s="143">
+      <c r="C10" s="142">
         <f t="shared" ref="C10:D10" si="1">C$8</f>
         <v>0</v>
       </c>
@@ -3672,21 +3672,21 @@
       <c r="A11" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="82">
+      <c r="B11" s="81">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C11" s="141">
-        <v>0</v>
-      </c>
-      <c r="D11" s="82" t="s">
+      <c r="C11" s="140">
+        <v>0</v>
+      </c>
+      <c r="D11" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
     </row>
     <row r="12" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
@@ -3696,7 +3696,7 @@
         <f>B11</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C12" s="142">
+      <c r="C12" s="141">
         <f>C11</f>
         <v>0</v>
       </c>
@@ -3719,7 +3719,7 @@
         <f>B11</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C13" s="143">
+      <c r="C13" s="142">
         <f>C11</f>
         <v>0</v>
       </c>
@@ -3738,21 +3738,21 @@
       <c r="A14" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="82">
+      <c r="B14" s="81">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C14" s="141">
-        <v>0</v>
-      </c>
-      <c r="D14" s="82" t="s">
+      <c r="C14" s="140">
+        <v>0</v>
+      </c>
+      <c r="D14" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
     </row>
     <row r="15" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
@@ -3762,7 +3762,7 @@
         <f>B14</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C15" s="142">
+      <c r="C15" s="141">
         <f>C14</f>
         <v>0</v>
       </c>
@@ -3785,7 +3785,7 @@
         <f>B14</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C16" s="143">
+      <c r="C16" s="142">
         <f>C14</f>
         <v>0</v>
       </c>
@@ -3804,13 +3804,13 @@
       <c r="A17" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="B17" s="82">
+      <c r="B17" s="81">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C17" s="141">
-        <v>0</v>
-      </c>
-      <c r="D17" s="82" t="s">
+      <c r="C17" s="140">
+        <v>0</v>
+      </c>
+      <c r="D17" s="81" t="s">
         <v>95</v>
       </c>
       <c r="E17" s="20"/>
@@ -3828,7 +3828,7 @@
         <f>B17</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C18" s="142">
+      <c r="C18" s="141">
         <f>C17</f>
         <v>0</v>
       </c>
@@ -3851,7 +3851,7 @@
         <f>B17</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C19" s="143">
+      <c r="C19" s="142">
         <f>C17</f>
         <v>0</v>
       </c>
@@ -3870,13 +3870,13 @@
       <c r="A20" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="B20" s="82">
+      <c r="B20" s="81">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C20" s="141">
-        <v>0</v>
-      </c>
-      <c r="D20" s="82" t="s">
+      <c r="C20" s="140">
+        <v>0</v>
+      </c>
+      <c r="D20" s="81" t="s">
         <v>95</v>
       </c>
       <c r="E20" s="20"/>
@@ -3894,7 +3894,7 @@
         <f>B20</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C21" s="142">
+      <c r="C21" s="141">
         <f>C20</f>
         <v>0</v>
       </c>
@@ -3917,7 +3917,7 @@
         <f>B20</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="C22" s="143">
+      <c r="C22" s="142">
         <f>C20</f>
         <v>0</v>
       </c>
@@ -4046,7 +4046,7 @@
       <c r="J32" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -4058,7 +4058,7 @@
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
     </row>
-    <row r="40" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -4071,7 +4071,7 @@
       <c r="J40" s="20"/>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
@@ -4114,7 +4114,7 @@
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="98" t="s">
         <v>56</v>
       </c>
       <c r="C1" s="54" t="s">
@@ -4168,7 +4168,7 @@
       <c r="E4" s="45"/>
       <c r="F4" s="45"/>
       <c r="G4" s="45"/>
-      <c r="H4" s="112"/>
+      <c r="H4" s="111"/>
       <c r="I4" s="45"/>
       <c r="J4" s="45"/>
     </row>
@@ -4191,7 +4191,7 @@
       <c r="F5" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="H5" s="90">
+      <c r="H5" s="89">
         <f>(25.3/4.6668)*Ref!B$18</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>213</v>
       </c>
       <c r="G6" s="21"/>
-      <c r="H6" s="90">
+      <c r="H6" s="89">
         <f>H5</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4248,7 +4248,7 @@
       <c r="F7" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="H7" s="78">
+      <c r="H7" s="77">
         <f>H5</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>213</v>
       </c>
       <c r="G8" s="42"/>
-      <c r="H8" s="90">
+      <c r="H8" s="89">
         <f>(25.3/4.6668)*Ref!B$18</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>213</v>
       </c>
       <c r="G9" s="21"/>
-      <c r="H9" s="90">
+      <c r="H9" s="89">
         <f>H8</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>213</v>
       </c>
       <c r="G10" s="38"/>
-      <c r="H10" s="78">
+      <c r="H10" s="77">
         <f>H8</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4342,10 +4342,10 @@
       <c r="A11" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="100">
+      <c r="B11" s="99">
         <v>0.9</v>
       </c>
-      <c r="C11" s="133">
+      <c r="C11" s="132">
         <v>0</v>
       </c>
       <c r="D11" s="42" t="s">
@@ -4358,7 +4358,7 @@
         <v>213</v>
       </c>
       <c r="G11" s="42"/>
-      <c r="H11" s="90">
+      <c r="H11" s="89">
         <f>(25.3/4.6668)*Ref!B$18</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>213</v>
       </c>
       <c r="G12" s="27"/>
-      <c r="H12" s="90">
+      <c r="H12" s="89">
         <f>H11</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>213</v>
       </c>
       <c r="G13" s="38"/>
-      <c r="H13" s="78">
+      <c r="H13" s="77">
         <f>H11</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4423,10 +4423,10 @@
       <c r="A14" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="100">
+      <c r="B14" s="99">
         <v>0.9</v>
       </c>
-      <c r="C14" s="134">
+      <c r="C14" s="133">
         <v>0</v>
       </c>
       <c r="D14" s="42" t="s">
@@ -4439,7 +4439,7 @@
         <v>213</v>
       </c>
       <c r="G14" s="42"/>
-      <c r="H14" s="90">
+      <c r="H14" s="89">
         <f>(25.3/4.6668)*Ref!B$18</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>213</v>
       </c>
       <c r="G15" s="21"/>
-      <c r="H15" s="90">
+      <c r="H15" s="89">
         <f>H14</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>213</v>
       </c>
       <c r="G16" s="38"/>
-      <c r="H16" s="78">
+      <c r="H16" s="77">
         <f>H14</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4507,10 +4507,10 @@
       <c r="A17" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="100">
+      <c r="B17" s="99">
         <v>0.9</v>
       </c>
-      <c r="C17" s="134">
+      <c r="C17" s="133">
         <v>0</v>
       </c>
       <c r="D17" s="42" t="s">
@@ -4522,7 +4522,7 @@
       <c r="F17" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="H17" s="90">
+      <c r="H17" s="89">
         <f>(25.3/4.6668)*Ref!B$18</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>213</v>
       </c>
       <c r="G18" s="21"/>
-      <c r="H18" s="90">
+      <c r="H18" s="89">
         <f>H17</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>213</v>
       </c>
       <c r="G19" s="38"/>
-      <c r="H19" s="78">
+      <c r="H19" s="77">
         <f>H17</f>
         <v>1.9516585240421703E-2</v>
       </c>
@@ -4633,87 +4633,87 @@
     <col min="1" max="1" width="26.42578125" style="21" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="21" customWidth="1"/>
     <col min="3" max="5" width="8.85546875" style="21"/>
-    <col min="6" max="6" width="8.85546875" style="96"/>
+    <col min="6" max="6" width="8.85546875" style="95"/>
     <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="D1" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="101" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="101" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="105" t="s">
+      <c r="D2" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="114" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="106"/>
+      <c r="G2" s="105"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="104" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="106"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="105"/>
     </row>
     <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="109">
+      <c r="B4" s="108">
         <v>1</v>
       </c>
-      <c r="C4" s="110">
+      <c r="C4" s="109">
         <v>0.9</v>
       </c>
-      <c r="D4" s="110">
+      <c r="D4" s="109">
         <v>1.05</v>
       </c>
-      <c r="E4" s="110">
+      <c r="E4" s="109">
         <v>0</v>
       </c>
       <c r="F4" s="29"/>
-      <c r="G4" s="111" t="s">
+      <c r="G4" s="110" t="s">
         <v>88</v>
       </c>
     </row>
@@ -4739,7 +4739,7 @@
         <f>0.001</f>
         <v>1E-3</v>
       </c>
-      <c r="G5" s="105"/>
+      <c r="G5" s="104"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
@@ -4761,7 +4761,7 @@
         <f t="shared" si="0"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="F6" s="135">
+      <c r="F6" s="134">
         <f>F5</f>
         <v>1E-3</v>
       </c>
@@ -4786,32 +4786,32 @@
         <f t="shared" si="1"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="F7" s="136">
+      <c r="F7" s="135">
         <f>F5</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="79" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="107">
+      <c r="B8" s="106">
         <v>1</v>
       </c>
-      <c r="C8" s="107">
+      <c r="C8" s="106">
         <v>0.9</v>
       </c>
       <c r="D8" s="47">
         <v>0.62</v>
       </c>
-      <c r="E8" s="107">
+      <c r="E8" s="106">
         <v>0</v>
       </c>
       <c r="F8" s="22">
         <f>0.001</f>
         <v>1E-3</v>
       </c>
-      <c r="G8" s="108"/>
+      <c r="G8" s="107"/>
     </row>
     <row r="9" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
@@ -4833,7 +4833,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F9" s="135">
+      <c r="F9" s="134">
         <f>F8</f>
         <v>1E-3</v>
       </c>
@@ -4859,7 +4859,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F10" s="136">
+      <c r="F10" s="135">
         <f>F8</f>
         <v>1E-3</v>
       </c>
@@ -4933,7 +4933,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F13" s="114">
+      <c r="F13" s="113">
         <f>F11</f>
         <v>0</v>
       </c>
@@ -4961,7 +4961,7 @@
         <f>0.001</f>
         <v>1E-3</v>
       </c>
-      <c r="G14" s="105" t="s">
+      <c r="G14" s="104" t="s">
         <v>211</v>
       </c>
     </row>
@@ -5010,7 +5010,7 @@
         <f t="shared" si="7"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="F16" s="114">
+      <c r="F16" s="113">
         <f>F14</f>
         <v>1E-3</v>
       </c>
@@ -5101,7 +5101,7 @@
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="96"/>
+      <c r="F21" s="95"/>
       <c r="G21" s="21"/>
     </row>
     <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -5110,16 +5110,16 @@
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="96"/>
+      <c r="F25" s="95"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="107" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
-      <c r="F33" s="96"/>
+      <c r="F33" s="95"/>
       <c r="G33" s="21"/>
     </row>
     <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -5128,7 +5128,7 @@
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
-      <c r="F37" s="96"/>
+      <c r="F37" s="95"/>
       <c r="G37" s="21"/>
     </row>
   </sheetData>
@@ -5153,87 +5153,87 @@
     <col min="1" max="1" width="26.42578125" style="21" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="21" customWidth="1"/>
     <col min="3" max="5" width="8.85546875" style="21"/>
-    <col min="6" max="6" width="8.85546875" style="96"/>
+    <col min="6" max="6" width="8.85546875" style="95"/>
     <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="D1" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="101" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="101" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="105" t="s">
+      <c r="D2" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="114" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="106"/>
+      <c r="G2" s="105"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="104" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="106"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="105"/>
     </row>
     <row r="4" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="109">
+      <c r="B4" s="108">
         <v>1</v>
       </c>
-      <c r="C4" s="110">
+      <c r="C4" s="109">
         <v>0.9</v>
       </c>
-      <c r="D4" s="110">
+      <c r="D4" s="109">
         <v>1.05</v>
       </c>
-      <c r="E4" s="110">
+      <c r="E4" s="109">
         <v>0</v>
       </c>
       <c r="F4" s="29"/>
-      <c r="G4" s="111"/>
+      <c r="G4" s="110"/>
     </row>
     <row r="5" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -5257,7 +5257,7 @@
         <f>0.001</f>
         <v>1E-3</v>
       </c>
-      <c r="G5" s="105"/>
+      <c r="G5" s="104"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
@@ -5279,7 +5279,7 @@
         <f t="shared" si="0"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="F6" s="135">
+      <c r="F6" s="134">
         <f>F5</f>
         <v>1E-3</v>
       </c>
@@ -5304,13 +5304,13 @@
         <f t="shared" si="1"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="F7" s="136">
+      <c r="F7" s="135">
         <f>F5</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="79" t="s">
         <v>119</v>
       </c>
       <c r="B8" s="47">
@@ -5331,7 +5331,7 @@
         <f>0.001</f>
         <v>1E-3</v>
       </c>
-      <c r="G8" s="108"/>
+      <c r="G8" s="107"/>
     </row>
     <row r="9" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
@@ -5353,7 +5353,7 @@
         <f t="shared" si="2"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="F9" s="135">
+      <c r="F9" s="134">
         <f>F8</f>
         <v>1E-3</v>
       </c>
@@ -5379,7 +5379,7 @@
         <f t="shared" si="3"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="F10" s="136">
+      <c r="F10" s="135">
         <f>F8</f>
         <v>1E-3</v>
       </c>
@@ -5452,7 +5452,7 @@
         <f t="shared" si="5"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="F13" s="114">
+      <c r="F13" s="113">
         <f>F11</f>
         <v>1E-3</v>
       </c>
@@ -5480,7 +5480,7 @@
         <f>0.001</f>
         <v>1E-3</v>
       </c>
-      <c r="G14" s="105"/>
+      <c r="G14" s="104"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
@@ -5527,7 +5527,7 @@
         <f t="shared" si="7"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="F16" s="114">
+      <c r="F16" s="113">
         <f>F14</f>
         <v>1E-3</v>
       </c>
@@ -5613,7 +5613,7 @@
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="96"/>
+      <c r="F21" s="95"/>
       <c r="G21" s="21"/>
     </row>
     <row r="25" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -5622,16 +5622,16 @@
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="96"/>
+      <c r="F25" s="95"/>
       <c r="G25" s="21"/>
     </row>
-    <row r="33" spans="1:7" s="108" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="107" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
-      <c r="F33" s="96"/>
+      <c r="F33" s="95"/>
       <c r="G33" s="21"/>
     </row>
     <row r="37" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -5640,7 +5640,7 @@
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
-      <c r="F37" s="96"/>
+      <c r="F37" s="95"/>
       <c r="G37" s="21"/>
     </row>
   </sheetData>
@@ -5660,44 +5660,44 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="100" t="s">
         <v>209</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="101" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="103" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="104" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="106"/>
+      <c r="C3" s="105"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="108" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="47">
         <v>0</v>
       </c>
-      <c r="C4" s="110">
+      <c r="C4" s="109">
         <v>0.32</v>
       </c>
     </row>
@@ -5740,7 +5740,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="79" t="s">
         <v>119</v>
       </c>
       <c r="B8" s="47">
@@ -5911,7 +5911,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="100" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -5928,7 +5928,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="102" t="s">
         <v>72</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -5942,12 +5942,12 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="102" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="108" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="30">
@@ -6459,7 +6459,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="H16" s="122"/>
+      <c r="H16" s="121"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
@@ -6480,7 +6480,7 @@
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="23"/>
-      <c r="E18" s="122"/>
+      <c r="E18" s="121"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
@@ -6500,7 +6500,7 @@
         <f>1.163</f>
         <v>1.163</v>
       </c>
-      <c r="E20" s="122"/>
+      <c r="E20" s="121"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
@@ -6538,7 +6538,7 @@
     <col min="1" max="1" width="19.42578125" style="21" customWidth="1"/>
     <col min="2" max="2" width="26.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" style="81" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="80" customWidth="1"/>
     <col min="6" max="6" width="63.28515625" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
@@ -6553,10 +6553,10 @@
       <c r="C1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="80" t="s">
         <v>58</v>
       </c>
       <c r="F1" s="21" t="s">
@@ -6645,8 +6645,8 @@
         <f>30*Ref!$B$18</f>
         <v>0.108</v>
       </c>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -6819,7 +6819,7 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="81" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="80" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="21" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
@@ -6832,7 +6832,7 @@
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="80" t="s">
         <v>157</v>
       </c>
       <c r="C1" s="21" t="s">
@@ -6861,7 +6861,7 @@
       <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>158</v>
       </c>
       <c r="H2" s="21" t="s">
@@ -6872,7 +6872,7 @@
       <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="85"/>
+      <c r="B3" s="84"/>
     </row>
     <row r="4" spans="1:9" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
@@ -6903,7 +6903,7 @@
       <c r="A5" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="86">
+      <c r="B5" s="85">
         <v>0.72</v>
       </c>
       <c r="C5" s="57">
@@ -6932,7 +6932,7 @@
       <c r="A6" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="B6" s="86"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="22">
         <f>C$5</f>
         <v>2.7906976744186046E-2</v>
@@ -6962,7 +6962,7 @@
       <c r="A7" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="87"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="29">
         <f>C$5</f>
         <v>2.7906976744186046E-2</v>
@@ -6991,7 +6991,7 @@
       <c r="A8" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="86">
+      <c r="B8" s="85">
         <v>0.72</v>
       </c>
       <c r="C8" s="57">
@@ -7020,7 +7020,7 @@
       <c r="A9" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="86"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="22">
         <f>C8</f>
         <v>2.7906976744186046E-2</v>
@@ -7051,7 +7051,7 @@
       <c r="A10" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="87"/>
       <c r="C10" s="29">
         <f>C8</f>
         <v>2.7906976744186046E-2</v>
@@ -7080,7 +7080,7 @@
       <c r="A11" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="89">
+      <c r="B11" s="88">
         <v>0.72</v>
       </c>
       <c r="C11" s="57">
@@ -7106,7 +7106,7 @@
       <c r="A12" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="89"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="28">
         <f>C11</f>
         <v>2.6100000000000002E-2</v>
@@ -7136,7 +7136,7 @@
       <c r="A13" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="88"/>
+      <c r="B13" s="87"/>
       <c r="C13" s="39">
         <f>C11</f>
         <v>2.6100000000000002E-2</v>
@@ -7337,7 +7337,7 @@
     </row>
     <row r="21" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
-      <c r="B21" s="81"/>
+      <c r="B21" s="80"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -7348,7 +7348,7 @@
     </row>
     <row r="33" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
-      <c r="B33" s="81"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
@@ -7359,7 +7359,7 @@
     </row>
     <row r="37" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
-      <c r="B37" s="81"/>
+      <c r="B37" s="80"/>
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
@@ -7798,14 +7798,14 @@
       <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" style="21" customWidth="1"/>
     <col min="2" max="4" width="11.42578125" style="21"/>
-    <col min="5" max="6" width="0" style="129" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="0" style="128" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="21"/>
     <col min="8" max="8" width="11.42578125" style="27"/>
     <col min="9" max="9" width="9.85546875" style="21" customWidth="1"/>
@@ -7813,8 +7813,8 @@
     <col min="14" max="14" width="20.7109375" style="21" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" style="21" customWidth="1"/>
     <col min="16" max="16" width="11.42578125" style="21"/>
-    <col min="17" max="17" width="12.42578125" style="81" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="0" style="81" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="80" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="0" style="80" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="11.42578125" style="55"/>
     <col min="20" max="16384" width="11.42578125" style="21"/>
   </cols>
@@ -7832,10 +7832,10 @@
       <c r="D1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="124" t="s">
+      <c r="E1" s="123" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="124" t="s">
+      <c r="F1" s="123" t="s">
         <v>182</v>
       </c>
       <c r="G1" s="21" t="s">
@@ -7868,10 +7868,10 @@
       <c r="P1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="81" t="s">
+      <c r="Q1" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="81" t="s">
+      <c r="R1" s="80" t="s">
         <v>105</v>
       </c>
       <c r="S1" s="64" t="s">
@@ -7894,10 +7894,10 @@
       <c r="D2" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="125" t="s">
+      <c r="E2" s="124" t="s">
         <v>181</v>
       </c>
-      <c r="F2" s="125"/>
+      <c r="F2" s="124"/>
       <c r="G2" s="21" t="s">
         <v>55</v>
       </c>
@@ -7916,7 +7916,7 @@
       <c r="O2" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" s="85" t="s">
+      <c r="Q2" s="84" t="s">
         <v>54</v>
       </c>
     </row>
@@ -7927,8 +7927,8 @@
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
       <c r="D3" s="55"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
     </row>
     <row r="4" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
@@ -7944,8 +7944,8 @@
         <f>0.109*0.56</f>
         <v>6.1040000000000004E-2</v>
       </c>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
       <c r="G4" s="30">
         <v>0</v>
       </c>
@@ -7979,7 +7979,7 @@
       </c>
       <c r="Q4" s="37"/>
       <c r="R4" s="37"/>
-      <c r="S4" s="84"/>
+      <c r="S4" s="83"/>
     </row>
     <row r="5" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -7995,10 +7995,10 @@
         <f>0.0132*(55/100)</f>
         <v>7.2600000000000008E-3</v>
       </c>
-      <c r="E5" s="127">
-        <v>0</v>
-      </c>
-      <c r="F5" s="127">
+      <c r="E5" s="126">
+        <v>0</v>
+      </c>
+      <c r="F5" s="126">
         <f t="shared" ref="F5:F13" si="0">E5*0.477</f>
         <v>0</v>
       </c>
@@ -8057,10 +8057,10 @@
         <f>D$5</f>
         <v>7.2600000000000008E-3</v>
       </c>
-      <c r="E6" s="128">
-        <v>0</v>
-      </c>
-      <c r="F6" s="127">
+      <c r="E6" s="127">
+        <v>0</v>
+      </c>
+      <c r="F6" s="126">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -8086,7 +8086,7 @@
       <c r="L6" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="M6" s="90">
+      <c r="M6" s="89">
         <f>M$5</f>
         <v>0.152</v>
       </c>
@@ -8099,8 +8099,8 @@
       <c r="P6" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="80"/>
       <c r="S6" s="65">
         <f t="shared" ref="S6:S7" si="3">I6*28.2+M6*25.8</f>
         <v>13.926959999999999</v>
@@ -8122,10 +8122,10 @@
         <f>D$5</f>
         <v>7.2600000000000008E-3</v>
       </c>
-      <c r="E7" s="126">
-        <v>0</v>
-      </c>
-      <c r="F7" s="126">
+      <c r="E7" s="125">
+        <v>0</v>
+      </c>
+      <c r="F7" s="125">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -8151,7 +8151,7 @@
       <c r="L7" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="M7" s="78">
+      <c r="M7" s="77">
         <f>M$5</f>
         <v>0.152</v>
       </c>
@@ -8185,10 +8185,10 @@
         <f>0.006*(55/100)</f>
         <v>3.3000000000000004E-3</v>
       </c>
-      <c r="E8" s="127">
-        <v>0</v>
-      </c>
-      <c r="F8" s="127">
+      <c r="E8" s="126">
+        <v>0</v>
+      </c>
+      <c r="F8" s="126">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -8224,7 +8224,7 @@
       <c r="P8" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="S8" s="79">
+      <c r="S8" s="78">
         <f t="shared" ref="S8:S13" si="4">I8*28.2+M8*25.8</f>
         <v>11.0562</v>
       </c>
@@ -8246,10 +8246,10 @@
         <f t="shared" si="5"/>
         <v>3.3000000000000004E-3</v>
       </c>
-      <c r="E9" s="128">
-        <v>0</v>
-      </c>
-      <c r="F9" s="127">
+      <c r="E9" s="127">
+        <v>0</v>
+      </c>
+      <c r="F9" s="126">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -8257,7 +8257,7 @@
         <f t="shared" si="5"/>
         <v>0.12564</v>
       </c>
-      <c r="H9" s="91">
+      <c r="H9" s="90">
         <f t="shared" si="5"/>
         <v>0.36118927456054245</v>
       </c>
@@ -8274,7 +8274,7 @@
       <c r="L9" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="M9" s="90">
+      <c r="M9" s="89">
         <f>M8</f>
         <v>0.152</v>
       </c>
@@ -8287,9 +8287,9 @@
       <c r="P9" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="79">
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="78">
         <f t="shared" si="4"/>
         <v>11.0562</v>
       </c>
@@ -8310,10 +8310,10 @@
         <f>D8</f>
         <v>3.3000000000000004E-3</v>
       </c>
-      <c r="E10" s="126">
-        <v>0</v>
-      </c>
-      <c r="F10" s="126">
+      <c r="E10" s="125">
+        <v>0</v>
+      </c>
+      <c r="F10" s="125">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -8377,15 +8377,16 @@
         <f>(1.1+18*(56/100)+9*(0.477/0.44)*(56/100))/145</f>
         <v>0.11478495297805644</v>
       </c>
-      <c r="E11" s="127">
+      <c r="E11" s="126">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F11" s="127">
+      <c r="F11" s="126">
         <f t="shared" si="0"/>
         <v>4.2929999999999991E-3</v>
       </c>
-      <c r="G11" s="74">
-        <v>0.3</v>
+      <c r="G11" s="143">
+        <f>G5</f>
+        <v>0.37331999999999999</v>
       </c>
       <c r="H11" s="35">
         <f>3400/24/145</f>
@@ -8415,14 +8416,14 @@
       <c r="P11" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="Q11" s="92">
+      <c r="Q11" s="91">
         <f>12*Ref!C5</f>
         <v>8.5888069956277322E-3</v>
       </c>
       <c r="R11" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="S11" s="75">
+      <c r="S11" s="74">
         <f t="shared" si="4"/>
         <v>15.738</v>
       </c>
@@ -8444,16 +8445,16 @@
         <f>D11</f>
         <v>0.11478495297805644</v>
       </c>
-      <c r="E12" s="127">
+      <c r="E12" s="126">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F12" s="127">
+      <c r="F12" s="126">
         <f t="shared" si="0"/>
         <v>4.2929999999999991E-3</v>
       </c>
       <c r="G12" s="26">
         <f t="shared" si="6"/>
-        <v>0.3</v>
+        <v>0.37331999999999999</v>
       </c>
       <c r="H12" s="56">
         <f t="shared" si="6"/>
@@ -8489,8 +8490,8 @@
         <f>P11</f>
         <v>charcoal - IPCC</v>
       </c>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="81"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="80"/>
       <c r="S12" s="65">
         <f t="shared" si="4"/>
         <v>15.738</v>
@@ -8512,16 +8513,16 @@
         <f>D11</f>
         <v>0.11478495297805644</v>
       </c>
-      <c r="E13" s="127">
+      <c r="E13" s="126">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F13" s="127">
+      <c r="F13" s="126">
         <f t="shared" si="0"/>
         <v>4.2929999999999991E-3</v>
       </c>
       <c r="G13" s="21">
         <f t="shared" si="7"/>
-        <v>0.3</v>
+        <v>0.37331999999999999</v>
       </c>
       <c r="H13" s="22">
         <f t="shared" si="7"/>
@@ -8557,8 +8558,8 @@
         <f>P11</f>
         <v>charcoal - IPCC</v>
       </c>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="81"/>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="80"/>
       <c r="S13" s="65">
         <f t="shared" si="4"/>
         <v>15.738</v>
@@ -8567,15 +8568,15 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H14" s="21"/>
-      <c r="S14" s="118"/>
+      <c r="S14" s="117"/>
     </row>
     <row r="17" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="129"/>
+      <c r="E17" s="128"/>
+      <c r="F17" s="128"/>
       <c r="G17" s="21"/>
       <c r="H17" s="27"/>
       <c r="I17" s="21"/>
@@ -8586,8 +8587,8 @@
       <c r="N17" s="21"/>
       <c r="O17" s="21"/>
       <c r="P17" s="21"/>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="81"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="80"/>
       <c r="S17" s="55"/>
       <c r="T17" s="21"/>
     </row>
@@ -8596,8 +8597,8 @@
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
+      <c r="E21" s="128"/>
+      <c r="F21" s="128"/>
       <c r="G21" s="21"/>
       <c r="H21" s="27"/>
       <c r="I21" s="21"/>
@@ -8608,8 +8609,8 @@
       <c r="N21" s="21"/>
       <c r="O21" s="21"/>
       <c r="P21" s="21"/>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="81"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="80"/>
       <c r="S21" s="55"/>
       <c r="T21" s="21"/>
     </row>
@@ -8618,8 +8619,8 @@
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
-      <c r="E25" s="129"/>
-      <c r="F25" s="129"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
       <c r="G25" s="21"/>
       <c r="H25" s="27"/>
       <c r="I25" s="21"/>
@@ -8630,16 +8631,16 @@
       <c r="N25" s="21"/>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
-      <c r="Q25" s="81"/>
-      <c r="R25" s="81"/>
+      <c r="Q25" s="80"/>
+      <c r="R25" s="80"/>
       <c r="S25" s="55"/>
       <c r="T25" s="21"/>
     </row>
     <row r="29" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="124"/>
-      <c r="F29" s="124"/>
-      <c r="Q29" s="116"/>
-      <c r="R29" s="116"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="123"/>
+      <c r="Q29" s="115"/>
+      <c r="R29" s="115"/>
       <c r="S29" s="64"/>
     </row>
     <row r="33" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -8647,8 +8648,8 @@
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="129"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
       <c r="G33" s="21"/>
       <c r="H33" s="27"/>
       <c r="I33" s="21"/>
@@ -8659,8 +8660,8 @@
       <c r="N33" s="21"/>
       <c r="O33" s="21"/>
       <c r="P33" s="21"/>
-      <c r="Q33" s="81"/>
-      <c r="R33" s="81"/>
+      <c r="Q33" s="80"/>
+      <c r="R33" s="80"/>
       <c r="S33" s="55"/>
       <c r="T33" s="21"/>
     </row>
@@ -8669,8 +8670,8 @@
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
-      <c r="E34" s="129"/>
-      <c r="F34" s="129"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="128"/>
       <c r="G34" s="21"/>
       <c r="H34" s="27"/>
       <c r="I34" s="21"/>
@@ -8681,8 +8682,8 @@
       <c r="N34" s="21"/>
       <c r="O34" s="21"/>
       <c r="P34" s="21"/>
-      <c r="Q34" s="81"/>
-      <c r="R34" s="81"/>
+      <c r="Q34" s="80"/>
+      <c r="R34" s="80"/>
       <c r="S34" s="55"/>
       <c r="T34" s="21"/>
     </row>
@@ -8691,8 +8692,8 @@
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
       <c r="D41" s="21"/>
-      <c r="E41" s="129"/>
-      <c r="F41" s="129"/>
+      <c r="E41" s="128"/>
+      <c r="F41" s="128"/>
       <c r="G41" s="21"/>
       <c r="H41" s="27"/>
       <c r="I41" s="21"/>
@@ -8703,8 +8704,8 @@
       <c r="N41" s="21"/>
       <c r="O41" s="21"/>
       <c r="P41" s="21"/>
-      <c r="Q41" s="81"/>
-      <c r="R41" s="81"/>
+      <c r="Q41" s="80"/>
+      <c r="R41" s="80"/>
       <c r="S41" s="55"/>
       <c r="T41" s="21"/>
     </row>
@@ -8730,9 +8731,9 @@
   <cols>
     <col min="1" max="1" width="21.42578125" style="21" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="81" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="80" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="81" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="80" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" style="21" customWidth="1"/>
     <col min="8" max="8" width="18.140625" style="21" bestFit="1" customWidth="1"/>
@@ -8750,13 +8751,13 @@
       <c r="B1" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="80" t="s">
         <v>68</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="80" t="s">
         <v>124</v>
       </c>
       <c r="F1" s="21" t="s">
@@ -8791,7 +8792,7 @@
       <c r="B2" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="84" t="s">
         <v>69</v>
       </c>
       <c r="D2" s="21" t="s">
@@ -8811,13 +8812,13 @@
       <c r="B3" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="85"/>
+      <c r="C3" s="84"/>
     </row>
     <row r="4" spans="1:13" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="95">
+      <c r="B4" s="94">
         <f>SUM(C4:D4)</f>
         <v>1.1000000000000001</v>
       </c>
@@ -8858,7 +8859,7 @@
         <f>SUM(C5:D5)</f>
         <v>1.0908</v>
       </c>
-      <c r="C5" s="92">
+      <c r="C5" s="91">
         <f>0.9008</f>
         <v>0.90080000000000005</v>
       </c>
@@ -8866,7 +8867,7 @@
         <f>0.1169+0.0731</f>
         <v>0.19</v>
       </c>
-      <c r="E5" s="93">
+      <c r="E5" s="92">
         <f t="shared" ref="E5:E10" si="0">D5/B5</f>
         <v>0.17418408507517419</v>
       </c>
@@ -8904,7 +8905,7 @@
         <f>B5</f>
         <v>1.0908</v>
       </c>
-      <c r="C6" s="94">
+      <c r="C6" s="93">
         <f t="shared" ref="C6:L6" si="1">C$5</f>
         <v>0.90080000000000005</v>
       </c>
@@ -9002,7 +9003,7 @@
         <f t="shared" ref="B8" si="3">SUM(C8:D8)</f>
         <v>1.0908</v>
       </c>
-      <c r="C8" s="92">
+      <c r="C8" s="91">
         <f>0.9008</f>
         <v>0.90080000000000005</v>
       </c>
@@ -9010,7 +9011,7 @@
         <f>0.1169+0.0731</f>
         <v>0.19</v>
       </c>
-      <c r="E8" s="93">
+      <c r="E8" s="92">
         <f t="shared" si="0"/>
         <v>0.17418408507517419</v>
       </c>
@@ -9133,7 +9134,7 @@
         <f t="shared" si="5"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="L10" s="114">
+      <c r="L10" s="113">
         <f t="shared" si="5"/>
         <v>7.4236530739716242E-2</v>
       </c>
@@ -9146,7 +9147,7 @@
         <f>SUM(C11:D11)</f>
         <v>1.0908</v>
       </c>
-      <c r="C11" s="92">
+      <c r="C11" s="91">
         <f>0.9008</f>
         <v>0.90080000000000005</v>
       </c>
@@ -9154,7 +9155,7 @@
         <f>0.1169+0.0731</f>
         <v>0.19</v>
       </c>
-      <c r="E11" s="93">
+      <c r="E11" s="92">
         <f t="shared" ref="E11:E13" si="6">D11/B11</f>
         <v>0.17418408507517419</v>
       </c>
@@ -9285,9 +9286,9 @@
     <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
-      <c r="C14" s="81"/>
+      <c r="C14" s="80"/>
       <c r="D14" s="21"/>
-      <c r="E14" s="81"/>
+      <c r="E14" s="80"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
@@ -9300,9 +9301,9 @@
     <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
-      <c r="C18" s="81"/>
+      <c r="C18" s="80"/>
       <c r="D18" s="21"/>
-      <c r="E18" s="81"/>
+      <c r="E18" s="80"/>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -9315,9 +9316,9 @@
     <row r="22" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
-      <c r="C22" s="81"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="81"/>
+      <c r="E22" s="80"/>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
@@ -9330,9 +9331,9 @@
     <row r="26" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
-      <c r="C26" s="81"/>
+      <c r="C26" s="80"/>
       <c r="D26" s="21"/>
-      <c r="E26" s="81"/>
+      <c r="E26" s="80"/>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
@@ -9345,9 +9346,9 @@
     <row r="30" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
-      <c r="C30" s="81"/>
+      <c r="C30" s="80"/>
       <c r="D30" s="21"/>
-      <c r="E30" s="81"/>
+      <c r="E30" s="80"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -9360,9 +9361,9 @@
     <row r="34" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
-      <c r="C34" s="81"/>
+      <c r="C34" s="80"/>
       <c r="D34" s="21"/>
-      <c r="E34" s="81"/>
+      <c r="E34" s="80"/>
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
@@ -9375,9 +9376,9 @@
     <row r="38" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
-      <c r="C38" s="81"/>
+      <c r="C38" s="80"/>
       <c r="D38" s="21"/>
-      <c r="E38" s="81"/>
+      <c r="E38" s="80"/>
       <c r="F38" s="21"/>
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
@@ -9477,13 +9478,13 @@
       <c r="F2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="G2" s="137" t="s">
+      <c r="G2" s="136" t="s">
         <v>187</v>
       </c>
-      <c r="H2" s="137" t="s">
+      <c r="H2" s="136" t="s">
         <v>187</v>
       </c>
-      <c r="I2" s="137" t="s">
+      <c r="I2" s="136" t="s">
         <v>187</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -9495,13 +9496,13 @@
       <c r="L2" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="M2" s="137" t="s">
+      <c r="M2" s="136" t="s">
         <v>172</v>
       </c>
-      <c r="N2" s="137" t="s">
+      <c r="N2" s="136" t="s">
         <v>172</v>
       </c>
-      <c r="O2" s="137" t="s">
+      <c r="O2" s="136" t="s">
         <v>192</v>
       </c>
     </row>
@@ -9534,7 +9535,7 @@
       <c r="H4" s="36">
         <v>2.6949999999999998</v>
       </c>
-      <c r="I4" s="138"/>
+      <c r="I4" s="137"/>
       <c r="J4" s="18">
         <v>0.40333000000000002</v>
       </c>
@@ -9571,11 +9572,11 @@
         <f>G5+H5</f>
         <v>1.7271428571428573</v>
       </c>
-      <c r="H5" s="138">
+      <c r="H5" s="137">
         <f>2.418/1.4</f>
         <v>1.7271428571428573</v>
       </c>
-      <c r="I5" s="138">
+      <c r="I5" s="137">
         <f>1.195*1.3/1.4</f>
         <v>1.1096428571428574</v>
       </c>
@@ -9608,11 +9609,11 @@
         <f>G6+H6</f>
         <v>1.2030769230769232</v>
       </c>
-      <c r="H6" s="138">
+      <c r="H6" s="137">
         <f>1.564/1.3</f>
         <v>1.2030769230769232</v>
       </c>
-      <c r="I6" s="138">
+      <c r="I6" s="137">
         <f>0.954/1.3</f>
         <v>0.73384615384615381</v>
       </c>
@@ -9652,11 +9653,11 @@
         <f>G7+H7</f>
         <v>2.25</v>
       </c>
-      <c r="H7" s="138">
+      <c r="H7" s="137">
         <f>2.925/1.3</f>
         <v>2.25</v>
       </c>
-      <c r="I7" s="138">
+      <c r="I7" s="137">
         <v>0</v>
       </c>
       <c r="J7" s="18">
@@ -9675,7 +9676,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="139" t="s">
+      <c r="A8" s="138" t="s">
         <v>204</v>
       </c>
       <c r="B8" t="s">
@@ -9695,10 +9696,10 @@
         <f t="shared" ref="F8" si="0">G8+H8</f>
         <v>0.54300000000000004</v>
       </c>
-      <c r="H8" s="140">
+      <c r="H8" s="139">
         <v>0.54300000000000004</v>
       </c>
-      <c r="I8" s="138"/>
+      <c r="I8" s="137"/>
       <c r="J8" s="18">
         <f>0.0365*28</f>
         <v>1.022</v>
@@ -9708,7 +9709,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="139" t="s">
+      <c r="A9" s="138" t="s">
         <v>205</v>
       </c>
       <c r="B9" t="s">
@@ -9728,10 +9729,10 @@
         <f>G9+H9</f>
         <v>1.3819999999999999</v>
       </c>
-      <c r="H9" s="140">
+      <c r="H9" s="139">
         <v>1.3819999999999999</v>
       </c>
-      <c r="I9" s="138"/>
+      <c r="I9" s="137"/>
       <c r="J9" s="18">
         <f>0.047*28</f>
         <v>1.3160000000000001</v>
@@ -10159,7 +10160,7 @@
       <c r="O18"/>
     </row>
     <row r="19" spans="1:15" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="87" t="s">
         <v>156</v>
       </c>
       <c r="B19" s="30" t="str">
@@ -10614,7 +10615,7 @@
       <c r="B5" s="41">
         <v>0</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="75">
         <f>((433-3.5*((H5/(H5+I5)*100)-79*(H5/(H5+I5))-101*(I5/(H5+I5))))*Ref!B$18)*(H5+I5)</f>
         <v>1.4236200000000001</v>
       </c>
@@ -10651,7 +10652,7 @@
       <c r="B6" s="41">
         <v>0</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="75">
         <f>((433-3.5*((H6/(H6+I6)*100)-79*(H6/(H6+I6))-101*(I6/(H6+I6))))*Ref!B$18)*(H6+I6)</f>
         <v>1.4236200000000001</v>
       </c>
@@ -10689,7 +10690,7 @@
       <c r="B7" s="40">
         <v>0</v>
       </c>
-      <c r="C7" s="77">
+      <c r="C7" s="76">
         <f>((433-3.5*((H7/(H7+I7)*100)-79*(H7/(H7+I7))-101*(I7/(H7+I7))))*Ref!B$18)*(H7+I7)</f>
         <v>1.4236200000000001</v>
       </c>
@@ -10727,7 +10728,7 @@
       <c r="B8" s="43">
         <v>0</v>
       </c>
-      <c r="C8" s="76">
+      <c r="C8" s="75">
         <f>698.1*Ref!B$18</f>
         <v>2.5131600000000001</v>
       </c>
@@ -10752,7 +10753,7 @@
         <f>0.901</f>
         <v>0.90100000000000002</v>
       </c>
-      <c r="J8" s="91">
+      <c r="J8" s="90">
         <f>0.0125/1.0543</f>
         <v>1.1856207910461918E-2</v>
       </c>
@@ -10768,7 +10769,7 @@
       <c r="B9" s="43">
         <v>0</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="75">
         <f>C8</f>
         <v>2.5131600000000001</v>
       </c>
@@ -10794,7 +10795,7 @@
         <f>I8</f>
         <v>0.90100000000000002</v>
       </c>
-      <c r="J9" s="91">
+      <c r="J9" s="90">
         <f>J8</f>
         <v>1.1856207910461918E-2</v>
       </c>
@@ -10810,7 +10811,7 @@
       <c r="B10" s="44">
         <v>0</v>
       </c>
-      <c r="C10" s="77">
+      <c r="C10" s="76">
         <f>C8</f>
         <v>2.5131600000000001</v>
       </c>
@@ -10836,7 +10837,7 @@
         <f>I8</f>
         <v>0.90100000000000002</v>
       </c>
-      <c r="J10" s="117">
+      <c r="J10" s="116">
         <f>J8</f>
         <v>1.1856207910461918E-2</v>
       </c>
@@ -10852,7 +10853,7 @@
       <c r="B11" s="43">
         <v>0</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="75">
         <f>698.1*Ref!B$18</f>
         <v>2.5131600000000001</v>
       </c>
@@ -10875,7 +10876,7 @@
       <c r="I11" s="28">
         <v>0.90100000000000002</v>
       </c>
-      <c r="J11" s="91">
+      <c r="J11" s="90">
         <f>0.0125/1.0543</f>
         <v>1.1856207910461918E-2</v>
       </c>
@@ -10891,7 +10892,7 @@
       <c r="B12" s="43">
         <v>0</v>
       </c>
-      <c r="C12" s="76">
+      <c r="C12" s="75">
         <f>C11</f>
         <v>2.5131600000000001</v>
       </c>
@@ -10917,7 +10918,7 @@
         <f>I11</f>
         <v>0.90100000000000002</v>
       </c>
-      <c r="J12" s="91">
+      <c r="J12" s="90">
         <f>J11</f>
         <v>1.1856207910461918E-2</v>
       </c>
@@ -10933,7 +10934,7 @@
       <c r="B13" s="44">
         <v>0</v>
       </c>
-      <c r="C13" s="77">
+      <c r="C13" s="76">
         <f>C11</f>
         <v>2.5131600000000001</v>
       </c>
@@ -10959,7 +10960,7 @@
         <f>I11</f>
         <v>0.90100000000000002</v>
       </c>
-      <c r="J13" s="117">
+      <c r="J13" s="116">
         <f>J11</f>
         <v>1.1856207910461918E-2</v>
       </c>

</xml_diff>